<commit_message>
updated experiment6 power and temperature data
</commit_message>
<xml_diff>
--- a/experiments/09_power_eval_1/predictor_comp.xlsx
+++ b/experiments/09_power_eval_1/predictor_comp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_TEMP2\experiment_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B922BF3-60C4-4696-B664-EE95B575F541}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FEC553-EDFB-4974-A431-ADB95A167A93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{39932099-E81A-42DA-B46C-E67CD6F446DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{39932099-E81A-42DA-B46C-E67CD6F446DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>Instance</t>
   </si>
@@ -152,6 +152,9 @@
   <si>
     <t>Stddev %</t>
   </si>
+  <si>
+    <t>eik</t>
+  </si>
 </sst>
 </file>
 
@@ -223,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -495,28 +498,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -532,7 +513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -603,7 +584,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -645,10 +626,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -661,12 +642,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -693,13 +668,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -754,13 +729,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -815,13 +790,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -876,13 +851,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1233,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F54CD9-8BC1-4FC4-9F69-18244224CB36}">
-  <dimension ref="A1:X42"/>
+  <dimension ref="A1:X47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1477,55 +1452,55 @@
         <v>0.18760700577356218</v>
       </c>
       <c r="E8" s="18">
-        <f t="shared" ref="E8:E21" si="0">D8/C8</f>
+        <f t="shared" ref="E8:E26" si="0">D8/C8</f>
         <v>2.1644871156482927E-2</v>
       </c>
       <c r="F8" s="17">
-        <f t="shared" ref="F8:F21" si="1">$C$1+U8</f>
+        <f t="shared" ref="F8:F25" si="1">$C$1+U8</f>
         <v>8.3995216808206106</v>
       </c>
       <c r="G8" s="16">
-        <f t="shared" ref="G8:G21" si="2">$C8-F8</f>
+        <f t="shared" ref="G8:G25" si="2">$C8-F8</f>
         <v>0.26798224734998399</v>
       </c>
       <c r="H8" s="18">
-        <f t="shared" ref="H8:H21" si="3">1-F8/$C8</f>
+        <f t="shared" ref="H8:H25" si="3">1-F8/$C8</f>
         <v>3.0918041638147375E-2</v>
       </c>
       <c r="I8" s="17">
-        <f t="shared" ref="I8:I21" si="4">$C$1+V8</f>
+        <f t="shared" ref="I8:I25" si="4">$C$1+V8</f>
         <v>8.0903201423590723</v>
       </c>
       <c r="J8" s="16">
-        <f t="shared" ref="J8:J21" si="5">$C8-I8</f>
+        <f t="shared" ref="J8:J25" si="5">$C8-I8</f>
         <v>0.5771837858115223</v>
       </c>
       <c r="K8" s="18">
-        <f t="shared" ref="K8:K21" si="6">1-I8/$C8</f>
+        <f t="shared" ref="K8:K25" si="6">1-I8/$C8</f>
         <v>6.6591695901699555E-2</v>
       </c>
       <c r="L8" s="17">
-        <f t="shared" ref="L8:L21" si="7">$C$1+W8</f>
+        <f t="shared" ref="L8:L25" si="7">$C$1+W8</f>
         <v>8.3022451476388515</v>
       </c>
       <c r="M8" s="16">
-        <f t="shared" ref="M8:M21" si="8">$C8-L8</f>
+        <f t="shared" ref="M8:M25" si="8">$C8-L8</f>
         <v>0.3652587805317431</v>
       </c>
       <c r="N8" s="18">
-        <f t="shared" ref="N8:N21" si="9">1-L8/$C8</f>
+        <f t="shared" ref="N8:N25" si="9">1-L8/$C8</f>
         <v>4.2141172771159807E-2</v>
       </c>
       <c r="O8" s="16">
-        <f t="shared" ref="O8:O21" si="10">$C$1+X8</f>
+        <f t="shared" ref="O8:O25" si="10">$C$1+X8</f>
         <v>8.548766422999341</v>
       </c>
       <c r="P8" s="16">
-        <f t="shared" ref="P8:P21" si="11">$C8-O8</f>
+        <f t="shared" ref="P8:P25" si="11">$C8-O8</f>
         <v>0.11873750517125359</v>
       </c>
       <c r="Q8" s="19">
-        <f t="shared" ref="Q8:Q21" si="12">1-O8/$C8</f>
+        <f t="shared" ref="Q8:Q25" si="12">1-O8/$C8</f>
         <v>1.3699157930040284E-2</v>
       </c>
       <c r="U8" s="2">
@@ -1620,81 +1595,81 @@
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A10" s="20">
-        <v>2</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="21">
-        <v>8.1750590818363271</v>
-      </c>
-      <c r="D10" s="21">
-        <v>0.1491626477531128</v>
-      </c>
-      <c r="E10" s="23">
-        <f t="shared" si="0"/>
-        <v>1.8246063577023967E-2</v>
-      </c>
-      <c r="F10" s="22">
-        <f t="shared" si="1"/>
-        <v>8.0464580654359956</v>
-      </c>
-      <c r="G10" s="21">
-        <f t="shared" si="2"/>
-        <v>0.1286010164003315</v>
-      </c>
-      <c r="H10" s="23">
-        <f t="shared" si="3"/>
-        <v>1.5730897491133988E-2</v>
-      </c>
-      <c r="I10" s="22">
-        <f t="shared" si="4"/>
-        <v>7.222382373128303</v>
-      </c>
-      <c r="J10" s="21">
-        <f t="shared" si="5"/>
-        <v>0.95267670870802412</v>
-      </c>
-      <c r="K10" s="23">
-        <f t="shared" si="6"/>
-        <v>0.11653453500106425</v>
-      </c>
-      <c r="L10" s="22">
-        <f t="shared" si="7"/>
-        <v>7.6412987636335314</v>
-      </c>
-      <c r="M10" s="21">
-        <f t="shared" si="8"/>
-        <v>0.53376031820279568</v>
-      </c>
-      <c r="N10" s="23">
-        <f t="shared" si="9"/>
-        <v>6.5291310173980932E-2</v>
-      </c>
-      <c r="O10" s="21">
-        <f t="shared" si="10"/>
-        <v>8.762063786435192</v>
-      </c>
-      <c r="P10" s="21">
-        <f t="shared" si="11"/>
-        <v>-0.58700470459886489</v>
-      </c>
-      <c r="Q10" s="24">
-        <f t="shared" si="12"/>
-        <v>-7.1804337891954173E-2</v>
+      <c r="A10" s="15">
+        <v>1</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="16">
+        <v>7.7386565088757395</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0.30965242196380238</v>
+      </c>
+      <c r="E10" s="18">
+        <f t="shared" ref="E10" si="13">D10/C10</f>
+        <v>4.001371835132507E-2</v>
+      </c>
+      <c r="F10" s="17">
+        <f t="shared" ref="F10" si="14">$C$1+U10</f>
+        <v>7.6496578665211317</v>
+      </c>
+      <c r="G10" s="16">
+        <f t="shared" ref="G10" si="15">$C10-F10</f>
+        <v>8.899864235460786E-2</v>
+      </c>
+      <c r="H10" s="18">
+        <f t="shared" ref="H10" si="16">1-F10/$C10</f>
+        <v>1.150052883889241E-2</v>
+      </c>
+      <c r="I10" s="17">
+        <f t="shared" ref="I10" si="17">$C$1+V10</f>
+        <v>7.165627450051371</v>
+      </c>
+      <c r="J10" s="16">
+        <f t="shared" ref="J10" si="18">$C10-I10</f>
+        <v>0.5730290588243685</v>
+      </c>
+      <c r="K10" s="18">
+        <f t="shared" ref="K10" si="19">1-I10/$C10</f>
+        <v>7.4047615134118061E-2</v>
+      </c>
+      <c r="L10" s="17">
+        <f t="shared" ref="L10" si="20">$C$1+W10</f>
+        <v>7.5107729982431817</v>
+      </c>
+      <c r="M10" s="16">
+        <f t="shared" ref="M10" si="21">$C10-L10</f>
+        <v>0.22788351063255785</v>
+      </c>
+      <c r="N10" s="18">
+        <f t="shared" ref="N10" si="22">1-L10/$C10</f>
+        <v>2.9447425450553344E-2</v>
+      </c>
+      <c r="O10" s="16">
+        <f t="shared" ref="O10" si="23">$C$1+X10</f>
+        <v>8.4781679796618405</v>
+      </c>
+      <c r="P10" s="16">
+        <f t="shared" ref="P10" si="24">$C10-O10</f>
+        <v>-0.73951147078610102</v>
+      </c>
+      <c r="Q10" s="19">
+        <f t="shared" ref="Q10" si="25">1-O10/$C10</f>
+        <v>-9.5560704876606062E-2</v>
       </c>
       <c r="U10" s="2">
-        <v>2.3504513846153845</v>
+        <v>1.9536511857005201</v>
       </c>
       <c r="V10" s="2">
-        <v>1.5263756923076923</v>
+        <v>1.4696207692307599</v>
       </c>
       <c r="W10" s="2">
-        <v>1.9452920828129201</v>
+        <v>1.8147663174225701</v>
       </c>
       <c r="X10" s="2">
-        <v>3.06605710561458</v>
+        <v>2.7821612988412299</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
@@ -1702,77 +1677,77 @@
         <v>2</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="21">
-        <v>8.9225564444444441</v>
+        <v>8.1750590818363271</v>
       </c>
       <c r="D11" s="21">
-        <v>0.15696522303890859</v>
+        <v>0.1491626477531128</v>
       </c>
       <c r="E11" s="23">
         <f t="shared" si="0"/>
-        <v>1.7591956298202146E-2</v>
+        <v>1.8246063577023967E-2</v>
       </c>
       <c r="F11" s="22">
         <f t="shared" si="1"/>
-        <v>8.4379379115898416</v>
+        <v>8.0464580654359956</v>
       </c>
       <c r="G11" s="21">
         <f t="shared" si="2"/>
-        <v>0.48461853285460244</v>
+        <v>0.1286010164003315</v>
       </c>
       <c r="H11" s="23">
         <f t="shared" si="3"/>
-        <v>5.4313865748234713E-2</v>
+        <v>1.5730897491133988E-2</v>
       </c>
       <c r="I11" s="22">
         <f t="shared" si="4"/>
-        <v>7.8964122962052272</v>
+        <v>7.222382373128303</v>
       </c>
       <c r="J11" s="21">
         <f t="shared" si="5"/>
-        <v>1.0261441482392168</v>
+        <v>0.95267670870802412</v>
       </c>
       <c r="K11" s="23">
         <f t="shared" si="6"/>
-        <v>0.11500562138535275</v>
+        <v>0.11653453500106425</v>
       </c>
       <c r="L11" s="22">
         <f t="shared" si="7"/>
-        <v>8.2167122126762209</v>
+        <v>7.6412987636335314</v>
       </c>
       <c r="M11" s="21">
         <f t="shared" si="8"/>
-        <v>0.7058442317682232</v>
+        <v>0.53376031820279568</v>
       </c>
       <c r="N11" s="23">
         <f t="shared" si="9"/>
-        <v>7.9107847191901115E-2</v>
+        <v>6.5291310173980932E-2</v>
       </c>
       <c r="O11" s="21">
         <f t="shared" si="10"/>
-        <v>8.6163971855051908</v>
+        <v>8.762063786435192</v>
       </c>
       <c r="P11" s="21">
         <f t="shared" si="11"/>
-        <v>0.30615925893925322</v>
+        <v>-0.58700470459886489</v>
       </c>
       <c r="Q11" s="24">
         <f t="shared" si="12"/>
-        <v>3.4312952890298676E-2</v>
+        <v>-7.1804337891954173E-2</v>
       </c>
       <c r="U11" s="2">
-        <v>2.741931230769231</v>
+        <v>2.3504513846153845</v>
       </c>
       <c r="V11" s="2">
-        <v>2.2004056153846157</v>
+        <v>1.5263756923076923</v>
       </c>
       <c r="W11" s="2">
-        <v>2.5207055318556102</v>
+        <v>1.9452920828129201</v>
       </c>
       <c r="X11" s="2">
-        <v>2.9203905046845802</v>
+        <v>3.06605710561458</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
@@ -1780,233 +1755,233 @@
         <v>2</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="21">
-        <v>7.8098835509138373</v>
+        <v>8.9225564444444441</v>
       </c>
       <c r="D12" s="21">
-        <v>0.28140906830485357</v>
+        <v>0.15696522303890859</v>
       </c>
       <c r="E12" s="23">
         <f t="shared" si="0"/>
-        <v>3.6032428200792548E-2</v>
+        <v>1.7591956298202146E-2</v>
       </c>
       <c r="F12" s="22">
         <f t="shared" si="1"/>
-        <v>7.5472798346667656</v>
+        <v>8.4379379115898416</v>
       </c>
       <c r="G12" s="21">
         <f t="shared" si="2"/>
-        <v>0.26260371624707179</v>
+        <v>0.48461853285460244</v>
       </c>
       <c r="H12" s="23">
         <f t="shared" si="3"/>
-        <v>3.3624536721337472E-2</v>
+        <v>5.4313865748234713E-2</v>
       </c>
       <c r="I12" s="22">
         <f t="shared" si="4"/>
-        <v>7.166231065435996</v>
+        <v>7.8964122962052272</v>
       </c>
       <c r="J12" s="21">
         <f t="shared" si="5"/>
-        <v>0.64365248547784137</v>
+        <v>1.0261441482392168</v>
       </c>
       <c r="K12" s="23">
         <f t="shared" si="6"/>
-        <v>8.2415119416540783E-2</v>
+        <v>0.11500562138535275</v>
       </c>
       <c r="L12" s="22">
         <f t="shared" si="7"/>
-        <v>7.5991695113384514</v>
+        <v>8.2167122126762209</v>
       </c>
       <c r="M12" s="21">
         <f t="shared" si="8"/>
-        <v>0.21071403957538593</v>
+        <v>0.7058442317682232</v>
       </c>
       <c r="N12" s="23">
         <f t="shared" si="9"/>
-        <v>2.698043296058239E-2</v>
+        <v>7.9107847191901115E-2</v>
       </c>
       <c r="O12" s="21">
         <f t="shared" si="10"/>
-        <v>8.6191512358207607</v>
+        <v>8.6163971855051908</v>
       </c>
       <c r="P12" s="21">
         <f t="shared" si="11"/>
-        <v>-0.80926768490692336</v>
+        <v>0.30615925893925322</v>
       </c>
       <c r="Q12" s="24">
         <f t="shared" si="12"/>
+        <v>3.4312952890298676E-2</v>
+      </c>
+      <c r="U12" s="2">
+        <v>2.741931230769231</v>
+      </c>
+      <c r="V12" s="2">
+        <v>2.2004056153846157</v>
+      </c>
+      <c r="W12" s="2">
+        <v>2.5207055318556102</v>
+      </c>
+      <c r="X12" s="2">
+        <v>2.9203905046845802</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13" s="20">
+        <v>2</v>
+      </c>
+      <c r="B13" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="21">
+        <v>7.8098835509138373</v>
+      </c>
+      <c r="D13" s="21">
+        <v>0.28140906830485357</v>
+      </c>
+      <c r="E13" s="23">
+        <f t="shared" si="0"/>
+        <v>3.6032428200792548E-2</v>
+      </c>
+      <c r="F13" s="22">
+        <f t="shared" si="1"/>
+        <v>7.5472798346667656</v>
+      </c>
+      <c r="G13" s="21">
+        <f t="shared" si="2"/>
+        <v>0.26260371624707179</v>
+      </c>
+      <c r="H13" s="23">
+        <f t="shared" si="3"/>
+        <v>3.3624536721337472E-2</v>
+      </c>
+      <c r="I13" s="22">
+        <f t="shared" si="4"/>
+        <v>7.166231065435996</v>
+      </c>
+      <c r="J13" s="21">
+        <f t="shared" si="5"/>
+        <v>0.64365248547784137</v>
+      </c>
+      <c r="K13" s="23">
+        <f t="shared" si="6"/>
+        <v>8.2415119416540783E-2</v>
+      </c>
+      <c r="L13" s="22">
+        <f t="shared" si="7"/>
+        <v>7.5991695113384514</v>
+      </c>
+      <c r="M13" s="21">
+        <f t="shared" si="8"/>
+        <v>0.21071403957538593</v>
+      </c>
+      <c r="N13" s="23">
+        <f t="shared" si="9"/>
+        <v>2.698043296058239E-2</v>
+      </c>
+      <c r="O13" s="21">
+        <f t="shared" si="10"/>
+        <v>8.6191512358207607</v>
+      </c>
+      <c r="P13" s="21">
+        <f t="shared" si="11"/>
+        <v>-0.80926768490692336</v>
+      </c>
+      <c r="Q13" s="24">
+        <f t="shared" si="12"/>
         <v>-0.103620966898057</v>
       </c>
-      <c r="U12" s="2">
+      <c r="U13" s="2">
         <v>1.851273153846154</v>
       </c>
-      <c r="V12" s="2">
+      <c r="V13" s="2">
         <v>1.4702243846153848</v>
       </c>
-      <c r="W12" s="2">
+      <c r="W13" s="2">
         <v>1.9031628305178401</v>
       </c>
-      <c r="X12" s="2">
+      <c r="X13" s="2">
         <v>2.92314455500015</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A13" s="25">
-        <v>3</v>
-      </c>
-      <c r="B13" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="26">
-        <v>8.1864021653543304</v>
-      </c>
-      <c r="D13" s="26">
-        <v>0.30290167558805503</v>
-      </c>
-      <c r="E13" s="28">
-        <f t="shared" si="0"/>
-        <v>3.7000585784798735E-2</v>
-      </c>
-      <c r="F13" s="27">
-        <f t="shared" si="1"/>
-        <v>8.1256968346667655</v>
-      </c>
-      <c r="G13" s="26">
-        <f t="shared" si="2"/>
-        <v>6.0705330687564896E-2</v>
-      </c>
-      <c r="H13" s="28">
-        <f t="shared" si="3"/>
-        <v>7.4153858387846494E-3</v>
-      </c>
-      <c r="I13" s="27">
-        <f t="shared" si="4"/>
-        <v>7.4797047577436881</v>
-      </c>
-      <c r="J13" s="26">
-        <f t="shared" si="5"/>
-        <v>0.70669740761064226</v>
-      </c>
-      <c r="K13" s="28">
-        <f t="shared" si="6"/>
-        <v>8.6325762323460786E-2</v>
-      </c>
-      <c r="L13" s="27">
-        <f t="shared" si="7"/>
-        <v>7.9129264232162813</v>
-      </c>
-      <c r="M13" s="26">
-        <f t="shared" si="8"/>
-        <v>0.27347574213804915</v>
-      </c>
-      <c r="N13" s="28">
-        <f t="shared" si="9"/>
-        <v>3.3406096672775942E-2</v>
-      </c>
-      <c r="O13" s="26">
-        <f t="shared" si="10"/>
-        <v>9.0543814225513906</v>
-      </c>
-      <c r="P13" s="26">
-        <f t="shared" si="11"/>
-        <v>-0.86797925719706015</v>
-      </c>
-      <c r="Q13" s="29">
-        <f t="shared" si="12"/>
-        <v>-0.10602695050463495</v>
-      </c>
-      <c r="U13" s="2">
-        <v>2.4296901538461535</v>
-      </c>
-      <c r="V13" s="2">
-        <v>1.7836980769230768</v>
-      </c>
-      <c r="W13" s="2">
-        <v>2.2169197423956701</v>
-      </c>
-      <c r="X13" s="2">
-        <v>3.3583747417307799</v>
-      </c>
-    </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A14" s="25">
-        <v>3</v>
-      </c>
-      <c r="B14" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="26">
-        <v>8.9912262443438919</v>
-      </c>
-      <c r="D14" s="26">
-        <v>0.24958836271839085</v>
-      </c>
-      <c r="E14" s="28">
-        <f t="shared" si="0"/>
-        <v>2.7759101588106443E-2</v>
-      </c>
-      <c r="F14" s="27">
-        <f t="shared" si="1"/>
-        <v>8.6220155269744581</v>
-      </c>
-      <c r="G14" s="26">
-        <f t="shared" si="2"/>
-        <v>0.36921071736943389</v>
-      </c>
-      <c r="H14" s="28">
-        <f t="shared" si="3"/>
-        <v>4.1063444221714818E-2</v>
-      </c>
-      <c r="I14" s="27">
-        <f t="shared" si="4"/>
-        <v>8.1140244500513816</v>
-      </c>
-      <c r="J14" s="26">
-        <f t="shared" si="5"/>
-        <v>0.87720179429251033</v>
-      </c>
-      <c r="K14" s="28">
-        <f t="shared" si="6"/>
-        <v>9.7561975469623086E-2</v>
-      </c>
-      <c r="L14" s="27">
-        <f t="shared" si="7"/>
-        <v>8.4903397637975715</v>
-      </c>
-      <c r="M14" s="26">
-        <f t="shared" si="8"/>
-        <v>0.50088648054632046</v>
-      </c>
-      <c r="N14" s="28">
-        <f t="shared" si="9"/>
-        <v>5.5708361344083968E-2</v>
-      </c>
-      <c r="O14" s="26">
-        <f t="shared" si="10"/>
-        <v>9.0195559095452715</v>
-      </c>
-      <c r="P14" s="26">
-        <f t="shared" si="11"/>
-        <v>-2.8329665201379584E-2</v>
-      </c>
-      <c r="Q14" s="29">
-        <f t="shared" si="12"/>
-        <v>-3.150812184177898E-3</v>
+      <c r="A14" s="20">
+        <v>2</v>
+      </c>
+      <c r="B14" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="21">
+        <v>8.0508098305084737</v>
+      </c>
+      <c r="D14" s="21">
+        <v>0.4134573880918902</v>
+      </c>
+      <c r="E14" s="23">
+        <f t="shared" ref="E14" si="26">D14/C14</f>
+        <v>5.135599980577072E-2</v>
+      </c>
+      <c r="F14" s="22">
+        <f t="shared" ref="F14" si="27">$C$1+U14</f>
+        <v>7.808873542709601</v>
+      </c>
+      <c r="G14" s="21">
+        <f t="shared" ref="G14" si="28">$C14-F14</f>
+        <v>0.24193628779887266</v>
+      </c>
+      <c r="H14" s="23">
+        <f t="shared" ref="H14" si="29">1-F14/$C14</f>
+        <v>3.0051174092084132E-2</v>
+      </c>
+      <c r="I14" s="22">
+        <f t="shared" ref="I14" si="30">$C$1+V14</f>
+        <v>7.1316789115898409</v>
+      </c>
+      <c r="J14" s="21">
+        <f t="shared" ref="J14" si="31">$C14-I14</f>
+        <v>0.91913091891863274</v>
+      </c>
+      <c r="K14" s="23">
+        <f t="shared" ref="K14" si="32">1-I14/$C14</f>
+        <v>0.11416626876908631</v>
+      </c>
+      <c r="L14" s="22">
+        <f t="shared" ref="L14" si="33">$C$1+W14</f>
+        <v>7.5485898544257211</v>
+      </c>
+      <c r="M14" s="21">
+        <f t="shared" ref="M14" si="34">$C14-L14</f>
+        <v>0.50221997608275259</v>
+      </c>
+      <c r="N14" s="23">
+        <f t="shared" ref="N14" si="35">1-L14/$C14</f>
+        <v>6.2381299106034627E-2</v>
+      </c>
+      <c r="O14" s="21">
+        <f t="shared" ref="O14" si="36">$C$1+X14</f>
+        <v>8.6991157235568117</v>
+      </c>
+      <c r="P14" s="21">
+        <f t="shared" ref="P14" si="37">$C14-O14</f>
+        <v>-0.64830589304833808</v>
+      </c>
+      <c r="Q14" s="24">
+        <f t="shared" ref="Q14" si="38">1-O14/$C14</f>
+        <v>-8.0526792545960957E-2</v>
       </c>
       <c r="U14" s="2">
-        <v>2.9260088461538465</v>
+        <v>2.1128668618889899</v>
       </c>
       <c r="V14" s="2">
-        <v>2.4180177692307696</v>
+        <v>1.43567223076923</v>
       </c>
       <c r="W14" s="2">
-        <v>2.7943330829769599</v>
+        <v>1.8525831736051099</v>
       </c>
       <c r="X14" s="2">
-        <v>3.32354922872466</v>
+        <v>3.0031090427362002</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
@@ -2014,857 +1989,1247 @@
         <v>3</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="26">
-        <v>8.1900440239043828</v>
+        <v>8.1864021653543304</v>
       </c>
       <c r="D15" s="26">
-        <v>0.20398054945489216</v>
+        <v>0.30290167558805503</v>
       </c>
       <c r="E15" s="28">
         <f t="shared" si="0"/>
-        <v>2.4905916117121178E-2</v>
+        <v>3.7000585784798735E-2</v>
       </c>
       <c r="F15" s="27">
         <f t="shared" si="1"/>
-        <v>7.7252361423590727</v>
+        <v>8.1256968346667655</v>
       </c>
       <c r="G15" s="26">
         <f t="shared" si="2"/>
-        <v>0.46480788154531005</v>
+        <v>6.0705330687564896E-2</v>
       </c>
       <c r="H15" s="28">
         <f t="shared" si="3"/>
-        <v>5.6752794025119901E-2</v>
+        <v>7.4153858387846494E-3</v>
       </c>
       <c r="I15" s="27">
         <f t="shared" si="4"/>
-        <v>7.25007545005138</v>
+        <v>7.4797047577436881</v>
       </c>
       <c r="J15" s="26">
         <f t="shared" si="5"/>
-        <v>0.93996857385300281</v>
+        <v>0.70669740761064226</v>
       </c>
       <c r="K15" s="28">
         <f t="shared" si="6"/>
-        <v>0.11476966071360606</v>
+        <v>8.6325762323460786E-2</v>
       </c>
       <c r="L15" s="27">
         <f t="shared" si="7"/>
-        <v>7.6968433632552316</v>
+        <v>7.9129264232162813</v>
       </c>
       <c r="M15" s="26">
         <f t="shared" si="8"/>
-        <v>0.49320066064915125</v>
+        <v>0.27347574213804915</v>
       </c>
       <c r="N15" s="28">
         <f t="shared" si="9"/>
-        <v>6.0219537185592698E-2</v>
+        <v>3.3406096672775942E-2</v>
       </c>
       <c r="O15" s="26">
         <f t="shared" si="10"/>
-        <v>8.9698741513115721</v>
+        <v>9.0543814225513906</v>
       </c>
       <c r="P15" s="26">
         <f t="shared" si="11"/>
-        <v>-0.77983012740718927</v>
+        <v>-0.86797925719706015</v>
       </c>
       <c r="Q15" s="29">
         <f t="shared" si="12"/>
+        <v>-0.10602695050463495</v>
+      </c>
+      <c r="U15" s="2">
+        <v>2.4296901538461535</v>
+      </c>
+      <c r="V15" s="2">
+        <v>1.7836980769230768</v>
+      </c>
+      <c r="W15" s="2">
+        <v>2.2169197423956701</v>
+      </c>
+      <c r="X15" s="2">
+        <v>3.3583747417307799</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16" s="25">
+        <v>3</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="26">
+        <v>8.9912262443438919</v>
+      </c>
+      <c r="D16" s="26">
+        <v>0.24958836271839085</v>
+      </c>
+      <c r="E16" s="28">
+        <f t="shared" si="0"/>
+        <v>2.7759101588106443E-2</v>
+      </c>
+      <c r="F16" s="27">
+        <f t="shared" si="1"/>
+        <v>8.6220155269744581</v>
+      </c>
+      <c r="G16" s="26">
+        <f t="shared" si="2"/>
+        <v>0.36921071736943389</v>
+      </c>
+      <c r="H16" s="28">
+        <f t="shared" si="3"/>
+        <v>4.1063444221714818E-2</v>
+      </c>
+      <c r="I16" s="27">
+        <f t="shared" si="4"/>
+        <v>8.1140244500513816</v>
+      </c>
+      <c r="J16" s="26">
+        <f t="shared" si="5"/>
+        <v>0.87720179429251033</v>
+      </c>
+      <c r="K16" s="28">
+        <f t="shared" si="6"/>
+        <v>9.7561975469623086E-2</v>
+      </c>
+      <c r="L16" s="27">
+        <f t="shared" si="7"/>
+        <v>8.4903397637975715</v>
+      </c>
+      <c r="M16" s="26">
+        <f t="shared" si="8"/>
+        <v>0.50088648054632046</v>
+      </c>
+      <c r="N16" s="28">
+        <f t="shared" si="9"/>
+        <v>5.5708361344083968E-2</v>
+      </c>
+      <c r="O16" s="26">
+        <f t="shared" si="10"/>
+        <v>9.0195559095452715</v>
+      </c>
+      <c r="P16" s="26">
+        <f t="shared" si="11"/>
+        <v>-2.8329665201379584E-2</v>
+      </c>
+      <c r="Q16" s="29">
+        <f t="shared" si="12"/>
+        <v>-3.150812184177898E-3</v>
+      </c>
+      <c r="U16" s="2">
+        <v>2.9260088461538465</v>
+      </c>
+      <c r="V16" s="2">
+        <v>2.4180177692307696</v>
+      </c>
+      <c r="W16" s="2">
+        <v>2.7943330829769599</v>
+      </c>
+      <c r="X16" s="2">
+        <v>3.32354922872466</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A17" s="25">
+        <v>3</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="26">
+        <v>8.1900440239043828</v>
+      </c>
+      <c r="D17" s="26">
+        <v>0.20398054945489216</v>
+      </c>
+      <c r="E17" s="28">
+        <f t="shared" si="0"/>
+        <v>2.4905916117121178E-2</v>
+      </c>
+      <c r="F17" s="27">
+        <f t="shared" si="1"/>
+        <v>7.7252361423590727</v>
+      </c>
+      <c r="G17" s="26">
+        <f t="shared" si="2"/>
+        <v>0.46480788154531005</v>
+      </c>
+      <c r="H17" s="28">
+        <f t="shared" si="3"/>
+        <v>5.6752794025119901E-2</v>
+      </c>
+      <c r="I17" s="27">
+        <f t="shared" si="4"/>
+        <v>7.25007545005138</v>
+      </c>
+      <c r="J17" s="26">
+        <f t="shared" si="5"/>
+        <v>0.93996857385300281</v>
+      </c>
+      <c r="K17" s="28">
+        <f t="shared" si="6"/>
+        <v>0.11476966071360606</v>
+      </c>
+      <c r="L17" s="27">
+        <f t="shared" si="7"/>
+        <v>7.6968433632552316</v>
+      </c>
+      <c r="M17" s="26">
+        <f t="shared" si="8"/>
+        <v>0.49320066064915125</v>
+      </c>
+      <c r="N17" s="28">
+        <f t="shared" si="9"/>
+        <v>6.0219537185592698E-2</v>
+      </c>
+      <c r="O17" s="26">
+        <f t="shared" si="10"/>
+        <v>8.9698741513115721</v>
+      </c>
+      <c r="P17" s="26">
+        <f t="shared" si="11"/>
+        <v>-0.77983012740718927</v>
+      </c>
+      <c r="Q17" s="29">
+        <f t="shared" si="12"/>
         <v>-9.5216841952386222E-2</v>
       </c>
-      <c r="U15" s="2">
+      <c r="U17" s="2">
         <v>2.0292294615384616</v>
       </c>
-      <c r="V15" s="2">
+      <c r="V17" s="2">
         <v>1.5540687692307693</v>
       </c>
-      <c r="W15" s="2">
+      <c r="W17" s="2">
         <v>2.00083668243462</v>
       </c>
-      <c r="X15" s="2">
+      <c r="X17" s="2">
         <v>3.2738674704909601</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A16" s="30">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A18" s="25">
+        <v>3</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="26">
+        <v>8.2021879799666113</v>
+      </c>
+      <c r="D18" s="26">
+        <v>0.33652739631399425</v>
+      </c>
+      <c r="E18" s="28">
+        <f t="shared" si="0"/>
+        <v>4.1028978747615116E-2</v>
+      </c>
+      <c r="F18" s="27">
+        <f t="shared" ref="F18" si="39">$C$1+U18</f>
+        <v>7.9040848469982414</v>
+      </c>
+      <c r="G18" s="26">
+        <f t="shared" ref="G18" si="40">$C18-F18</f>
+        <v>0.29810313296836988</v>
+      </c>
+      <c r="H18" s="28">
+        <f t="shared" ref="H18" si="41">1-F18/$C18</f>
+        <v>3.6344342960252796E-2</v>
+      </c>
+      <c r="I18" s="27">
+        <f t="shared" ref="I18" si="42">$C$1+V18</f>
+        <v>7.2377742192821408</v>
+      </c>
+      <c r="J18" s="26">
+        <f t="shared" ref="J18" si="43">$C18-I18</f>
+        <v>0.96441376068447049</v>
+      </c>
+      <c r="K18" s="28">
+        <f t="shared" ref="K18" si="44">1-I18/$C18</f>
+        <v>0.11758006071550631</v>
+      </c>
+      <c r="L18" s="27">
+        <f t="shared" ref="L18" si="45">$C$1+W18</f>
+        <v>7.6857938481775312</v>
+      </c>
+      <c r="M18" s="26">
+        <f t="shared" ref="M18" si="46">$C18-L18</f>
+        <v>0.51639413178908011</v>
+      </c>
+      <c r="N18" s="28">
+        <f t="shared" ref="N18" si="47">1-L18/$C18</f>
+        <v>6.2958095211953724E-2</v>
+      </c>
+      <c r="O18" s="26">
+        <f t="shared" ref="O18" si="48">$C$1+X18</f>
+        <v>8.9974887895323707</v>
+      </c>
+      <c r="P18" s="26">
+        <f t="shared" ref="P18" si="49">$C18-O18</f>
+        <v>-0.79530080956575944</v>
+      </c>
+      <c r="Q18" s="29">
+        <f t="shared" ref="Q18" si="50">1-O18/$C18</f>
+        <v>-9.6962031534541415E-2</v>
+      </c>
+      <c r="U18" s="2">
+        <v>2.2080781661776299</v>
+      </c>
+      <c r="V18" s="2">
+        <v>1.5417675384615299</v>
+      </c>
+      <c r="W18" s="2">
+        <v>1.9897871673569201</v>
+      </c>
+      <c r="X18" s="2">
+        <v>3.3014821087117601</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A19" s="30">
         <v>4</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="B19" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C19" s="31">
         <v>7.4630859289617479</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D19" s="31">
         <v>0.2783420640340748</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E19" s="33">
         <f t="shared" si="0"/>
         <v>3.7295840713011501E-2</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F19" s="32">
         <f t="shared" si="1"/>
         <v>8.0267967641539446</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G19" s="31">
         <f t="shared" si="2"/>
         <v>-0.56371083519219667</v>
       </c>
-      <c r="H16" s="33">
+      <c r="H19" s="33">
         <f t="shared" si="3"/>
         <v>-7.5533209795243472E-2</v>
       </c>
-      <c r="I16" s="32">
+      <c r="I19" s="32">
         <f t="shared" si="4"/>
         <v>7.134401680820611</v>
       </c>
-      <c r="J16" s="31">
+      <c r="J19" s="31">
         <f t="shared" si="5"/>
         <v>0.32868424814113695</v>
       </c>
-      <c r="K16" s="33">
+      <c r="K19" s="33">
         <f t="shared" si="6"/>
         <v>4.4041332401871802E-2</v>
       </c>
-      <c r="L16" s="32">
+      <c r="L19" s="32">
         <f t="shared" si="7"/>
         <v>7.5492793722859011</v>
       </c>
-      <c r="M16" s="31">
+      <c r="M19" s="31">
         <f t="shared" si="8"/>
         <v>-8.6193443324153129E-2</v>
       </c>
-      <c r="N16" s="33">
+      <c r="N19" s="33">
         <f t="shared" si="9"/>
         <v>-1.1549303350463225E-2</v>
       </c>
-      <c r="O16" s="31">
+      <c r="O19" s="31">
         <f t="shared" si="10"/>
         <v>8.3833663804523404</v>
       </c>
-      <c r="P16" s="31">
+      <c r="P19" s="31">
         <f t="shared" si="11"/>
         <v>-0.92028045149059245</v>
       </c>
-      <c r="Q16" s="34">
+      <c r="Q19" s="34">
         <f t="shared" si="12"/>
         <v>-0.12331098157657427</v>
       </c>
-      <c r="U16" s="2">
+      <c r="U19" s="2">
         <v>2.3307900833333335</v>
       </c>
-      <c r="V16" s="2">
+      <c r="V19" s="2">
         <v>1.4383950000000001</v>
       </c>
-      <c r="W16" s="2">
+      <c r="W19" s="2">
         <v>1.8532726914652899</v>
       </c>
-      <c r="X16" s="2">
+      <c r="X19" s="2">
         <v>2.6873596996317302</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A17" s="30">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A20" s="30">
         <v>4</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B20" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="31">
+      <c r="C20" s="31">
         <v>8.1467038674033159</v>
       </c>
-      <c r="D17" s="31">
+      <c r="D20" s="31">
         <v>0.20731566300858609</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E20" s="33">
         <f t="shared" si="0"/>
         <v>2.5447796603740549E-2</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F20" s="32">
         <f t="shared" si="1"/>
         <v>8.2816591808206113</v>
       </c>
-      <c r="G17" s="31">
+      <c r="G20" s="31">
         <f t="shared" si="2"/>
         <v>-0.13495531341729539</v>
       </c>
-      <c r="H17" s="33">
+      <c r="H20" s="33">
         <f t="shared" si="3"/>
         <v>-1.6565633858041773E-2</v>
       </c>
-      <c r="I17" s="32">
+      <c r="I20" s="32">
         <f t="shared" si="4"/>
         <v>7.9350504308206116</v>
       </c>
-      <c r="J17" s="31">
+      <c r="J20" s="31">
         <f t="shared" si="5"/>
         <v>0.2116534365827043</v>
       </c>
-      <c r="K17" s="33">
+      <c r="K20" s="33">
         <f t="shared" si="6"/>
         <v>2.5980254103696421E-2</v>
       </c>
-      <c r="L17" s="32">
+      <c r="L20" s="32">
         <f t="shared" si="7"/>
         <v>8.1284530422837307</v>
       </c>
-      <c r="M17" s="31">
+      <c r="M20" s="31">
         <f t="shared" si="8"/>
         <v>1.8250825119585201E-2</v>
       </c>
-      <c r="N17" s="33">
+      <c r="N20" s="33">
         <f t="shared" si="9"/>
         <v>2.240271085906409E-3</v>
       </c>
-      <c r="O17" s="31">
+      <c r="O20" s="31">
         <f t="shared" si="10"/>
         <v>8.3607343843141617</v>
       </c>
-      <c r="P17" s="31">
+      <c r="P20" s="31">
         <f t="shared" si="11"/>
         <v>-0.21403051691084585</v>
       </c>
-      <c r="Q17" s="34">
+      <c r="Q20" s="34">
         <f t="shared" si="12"/>
         <v>-2.6272038408960308E-2</v>
       </c>
-      <c r="U17" s="2">
+      <c r="U20" s="2">
         <v>2.5856525000000001</v>
       </c>
-      <c r="V17" s="2">
+      <c r="V20" s="2">
         <v>2.23904375</v>
       </c>
-      <c r="W17" s="2">
+      <c r="W20" s="2">
         <v>2.43244636146312</v>
       </c>
-      <c r="X17" s="2">
+      <c r="X20" s="2">
         <v>2.6647277034935501</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A18" s="30">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A21" s="30">
         <v>4</v>
       </c>
-      <c r="B18" s="52" t="s">
+      <c r="B21" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="31">
+      <c r="C21" s="31">
         <v>7.2364042292710069</v>
       </c>
-      <c r="D18" s="31">
+      <c r="D21" s="31">
         <v>0.27489160416221231</v>
       </c>
-      <c r="E18" s="33">
+      <c r="E21" s="33">
         <f t="shared" si="0"/>
         <v>3.7987320145865429E-2</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F21" s="32">
         <f t="shared" si="1"/>
         <v>7.4424792641539446</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G21" s="31">
         <f t="shared" si="2"/>
         <v>-0.20607503488293766</v>
       </c>
-      <c r="H18" s="33">
+      <c r="H21" s="33">
         <f t="shared" si="3"/>
         <v>-2.8477546078668592E-2</v>
       </c>
-      <c r="I18" s="32">
+      <c r="I21" s="32">
         <f t="shared" si="4"/>
         <v>7.0731279308206112</v>
       </c>
-      <c r="J18" s="31">
+      <c r="J21" s="31">
         <f t="shared" si="5"/>
         <v>0.16327629845039571</v>
       </c>
-      <c r="K18" s="33">
+      <c r="K21" s="33">
         <f t="shared" si="6"/>
         <v>2.2563181005000876E-2</v>
       </c>
-      <c r="L18" s="32">
+      <c r="L21" s="32">
         <f t="shared" si="7"/>
         <v>7.4170550388195613</v>
       </c>
-      <c r="M18" s="31">
+      <c r="M21" s="31">
         <f t="shared" si="8"/>
         <v>-0.18065080954855439</v>
       </c>
-      <c r="N18" s="33">
+      <c r="N21" s="33">
         <f t="shared" si="9"/>
         <v>-2.4964167813874782E-2</v>
       </c>
-      <c r="O18" s="31">
+      <c r="O21" s="31">
         <f t="shared" si="10"/>
         <v>8.2295084702911208</v>
       </c>
-      <c r="P18" s="31">
+      <c r="P21" s="31">
         <f t="shared" si="11"/>
         <v>-0.99310424102011385</v>
       </c>
-      <c r="Q18" s="34">
+      <c r="Q21" s="34">
         <f t="shared" si="12"/>
         <v>-0.13723725341420834</v>
       </c>
-      <c r="U18" s="2">
+      <c r="U21" s="2">
         <v>1.7464725833333334</v>
       </c>
-      <c r="V18" s="2">
+      <c r="V21" s="2">
         <v>1.3771212500000001</v>
       </c>
-      <c r="W18" s="2">
+      <c r="W21" s="2">
         <v>1.72104835799895</v>
       </c>
-      <c r="X18" s="2">
+      <c r="X21" s="2">
         <v>2.5335017894705101</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A19" s="35">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A22" s="30">
+        <v>4</v>
+      </c>
+      <c r="B22" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="31">
+        <v>7.7085365122615803</v>
+      </c>
+      <c r="D22" s="31">
+        <v>0.3752050982843535</v>
+      </c>
+      <c r="E22" s="33">
+        <f t="shared" si="0"/>
+        <v>4.8673973028153093E-2</v>
+      </c>
+      <c r="F22" s="32">
+        <f t="shared" ref="F22" si="51">$C$1+U22</f>
+        <v>7.5408011918333413</v>
+      </c>
+      <c r="G22" s="31">
+        <f t="shared" ref="G22" si="52">$C22-F22</f>
+        <v>0.16773532042823902</v>
+      </c>
+      <c r="H22" s="33">
+        <f t="shared" ref="H22" si="53">1-F22/$C22</f>
+        <v>2.1759684235967636E-2</v>
+      </c>
+      <c r="I22" s="32">
+        <f t="shared" ref="I22" si="54">$C$1+V22</f>
+        <v>7.0654755974872714</v>
+      </c>
+      <c r="J22" s="31">
+        <f t="shared" ref="J22" si="55">$C22-I22</f>
+        <v>0.64306091477430893</v>
+      </c>
+      <c r="K22" s="33">
+        <f t="shared" ref="K22" si="56">1-I22/$C22</f>
+        <v>8.3421919809476774E-2</v>
+      </c>
+      <c r="L22" s="32">
+        <f t="shared" ref="L22" si="57">$C$1+W22</f>
+        <v>7.3705687900295809</v>
+      </c>
+      <c r="M22" s="31">
+        <f t="shared" ref="M22" si="58">$C22-L22</f>
+        <v>0.33796772223199945</v>
+      </c>
+      <c r="N22" s="33">
+        <f t="shared" ref="N22" si="59">1-L22/$C22</f>
+        <v>4.3843305625446694E-2</v>
+      </c>
+      <c r="O22" s="31">
+        <f t="shared" ref="O22" si="60">$C$1+X22</f>
+        <v>8.2240995803169614</v>
+      </c>
+      <c r="P22" s="31">
+        <f t="shared" ref="P22" si="61">$C22-O22</f>
+        <v>-0.5155630680553811</v>
+      </c>
+      <c r="Q22" s="34">
+        <f t="shared" ref="Q22" si="62">1-O22/$C22</f>
+        <v>-6.6882094575968054E-2</v>
+      </c>
+      <c r="U22" s="2">
+        <v>1.84479451101273</v>
+      </c>
+      <c r="V22" s="2">
+        <v>1.36946891666666</v>
+      </c>
+      <c r="W22" s="2">
+        <v>1.67456210920897</v>
+      </c>
+      <c r="X22" s="2">
+        <v>2.5280928994963499</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A23" s="35">
         <v>5</v>
       </c>
-      <c r="B19" s="53" t="s">
+      <c r="B23" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="36">
+      <c r="C23" s="36">
         <v>8.199037379576108</v>
       </c>
-      <c r="D19" s="36">
+      <c r="D23" s="36">
         <v>0.25509964109722122</v>
       </c>
-      <c r="E19" s="38">
+      <c r="E23" s="38">
         <f t="shared" si="0"/>
         <v>3.1113364811907948E-2</v>
       </c>
-      <c r="F19" s="37">
+      <c r="F23" s="37">
         <f t="shared" si="1"/>
         <v>8.2131679885129181</v>
       </c>
-      <c r="G19" s="36">
+      <c r="G23" s="36">
         <f t="shared" si="2"/>
         <v>-1.4130608936810063E-2</v>
       </c>
-      <c r="H19" s="38">
+      <c r="H23" s="38">
         <f t="shared" si="3"/>
         <v>-1.7234473124869698E-3</v>
       </c>
-      <c r="I19" s="37">
+      <c r="I23" s="37">
         <f t="shared" si="4"/>
         <v>7.2936038346667651</v>
       </c>
-      <c r="J19" s="36">
+      <c r="J23" s="36">
         <f t="shared" si="5"/>
         <v>0.90543354490934291</v>
       </c>
-      <c r="K19" s="38">
+      <c r="K23" s="38">
         <f t="shared" si="6"/>
         <v>0.11043168886688914</v>
       </c>
-      <c r="L19" s="37">
+      <c r="L23" s="37">
         <f t="shared" si="7"/>
         <v>8.02679642725926</v>
       </c>
-      <c r="M19" s="36">
+      <c r="M23" s="36">
         <f t="shared" si="8"/>
         <v>0.172240952316848</v>
       </c>
-      <c r="N19" s="38">
+      <c r="N23" s="38">
         <f t="shared" si="9"/>
         <v>2.1007460308194448E-2</v>
       </c>
-      <c r="O19" s="36">
+      <c r="O23" s="36">
         <f t="shared" si="10"/>
         <v>9.3368600865873717</v>
       </c>
-      <c r="P19" s="36">
+      <c r="P23" s="36">
         <f t="shared" si="11"/>
         <v>-1.1378227070112636</v>
       </c>
-      <c r="Q19" s="39">
+      <c r="Q23" s="39">
         <f t="shared" si="12"/>
         <v>-0.13877515790397443</v>
       </c>
-      <c r="U19" s="2">
+      <c r="U23" s="2">
         <v>2.5171613076923078</v>
       </c>
-      <c r="V19" s="2">
+      <c r="V23" s="2">
         <v>1.5975971538461542</v>
       </c>
-      <c r="W19" s="2">
+      <c r="W23" s="2">
         <v>2.3307897464386498</v>
       </c>
-      <c r="X19" s="2">
+      <c r="X23" s="2">
         <v>3.6408534057667601</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A20" s="35">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A24" s="35">
         <v>5</v>
       </c>
-      <c r="B20" s="53" t="s">
+      <c r="B24" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="36">
+      <c r="C24" s="36">
         <v>8.5018009823182705</v>
       </c>
-      <c r="D20" s="36">
+      <c r="D24" s="36">
         <v>0.18190417941925968</v>
       </c>
-      <c r="E20" s="38">
+      <c r="E24" s="38">
         <f t="shared" si="0"/>
         <v>2.1395958314900248E-2</v>
       </c>
-      <c r="F20" s="37">
+      <c r="F24" s="37">
         <f t="shared" si="1"/>
         <v>8.6222809885129195</v>
       </c>
-      <c r="G20" s="36">
+      <c r="G24" s="36">
         <f t="shared" si="2"/>
         <v>-0.12048000619464894</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H24" s="38">
         <f t="shared" si="3"/>
         <v>-1.4171115795961198E-2</v>
       </c>
-      <c r="I20" s="37">
+      <c r="I24" s="37">
         <f t="shared" si="4"/>
         <v>8.008926373128304</v>
       </c>
-      <c r="J20" s="36">
+      <c r="J24" s="36">
         <f t="shared" si="5"/>
         <v>0.49287460918996651</v>
       </c>
-      <c r="K20" s="38">
+      <c r="K24" s="38">
         <f t="shared" si="6"/>
         <v>5.7972964812400218E-2</v>
       </c>
-      <c r="L20" s="37">
+      <c r="L24" s="37">
         <f t="shared" si="7"/>
         <v>8.4471994025161017</v>
       </c>
-      <c r="M20" s="36">
+      <c r="M24" s="36">
         <f t="shared" si="8"/>
         <v>5.4601579802168843E-2</v>
       </c>
-      <c r="N20" s="38">
+      <c r="N24" s="38">
         <f t="shared" si="9"/>
         <v>6.4223545006202309E-3</v>
       </c>
-      <c r="O20" s="36">
+      <c r="O24" s="36">
         <f t="shared" si="10"/>
         <v>9.0949931620531714</v>
       </c>
-      <c r="P20" s="36">
+      <c r="P24" s="36">
         <f t="shared" si="11"/>
         <v>-0.5931921797349009</v>
       </c>
-      <c r="Q20" s="39">
+      <c r="Q24" s="39">
         <f t="shared" si="12"/>
         <v>-6.9772531839853658E-2</v>
       </c>
-      <c r="U20" s="2">
+      <c r="U24" s="2">
         <v>2.9262743076923075</v>
       </c>
-      <c r="V20" s="2">
+      <c r="V24" s="2">
         <v>2.312919692307692</v>
       </c>
-      <c r="W20" s="2">
+      <c r="W24" s="2">
         <v>2.7511927216954901</v>
       </c>
-      <c r="X20" s="2">
+      <c r="X24" s="2">
         <v>3.3989864812325599</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="40">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A25" s="35">
         <v>5</v>
       </c>
-      <c r="B21" s="54" t="s">
+      <c r="B25" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="41">
+      <c r="C25" s="36">
         <v>8.0954876404494378</v>
       </c>
-      <c r="D21" s="41">
+      <c r="D25" s="36">
         <v>0.2954154330728892</v>
       </c>
-      <c r="E21" s="43">
+      <c r="E25" s="38">
         <f t="shared" si="0"/>
         <v>3.6491369784425812E-2</v>
       </c>
-      <c r="F21" s="42">
+      <c r="F25" s="37">
         <f t="shared" si="1"/>
         <v>7.7704354500513801</v>
       </c>
-      <c r="G21" s="41">
+      <c r="G25" s="36">
         <f t="shared" si="2"/>
         <v>0.32505219039805766</v>
       </c>
-      <c r="H21" s="43">
+      <c r="H25" s="38">
         <f t="shared" si="3"/>
         <v>4.0152268131930846E-2</v>
       </c>
-      <c r="I21" s="42">
+      <c r="I25" s="37">
         <f t="shared" si="4"/>
         <v>7.3088548346667652</v>
       </c>
-      <c r="J21" s="41">
+      <c r="J25" s="36">
         <f t="shared" si="5"/>
         <v>0.78663280578267258</v>
       </c>
-      <c r="K21" s="43">
+      <c r="K25" s="38">
         <f t="shared" si="6"/>
         <v>9.7169292415719255E-2</v>
       </c>
-      <c r="L21" s="42">
+      <c r="L25" s="37">
         <f t="shared" si="7"/>
         <v>7.6833852377524314</v>
       </c>
-      <c r="M21" s="41">
+      <c r="M25" s="36">
         <f t="shared" si="8"/>
         <v>0.41210240269700638</v>
       </c>
-      <c r="N21" s="43">
+      <c r="N25" s="38">
         <f t="shared" si="9"/>
         <v>5.0905198179528988E-2</v>
       </c>
-      <c r="O21" s="41">
+      <c r="O25" s="36">
         <f t="shared" si="10"/>
         <v>8.6625597651092612</v>
       </c>
-      <c r="P21" s="41">
+      <c r="P25" s="36">
         <f t="shared" si="11"/>
         <v>-0.56707212465982337</v>
       </c>
-      <c r="Q21" s="44">
+      <c r="Q25" s="39">
         <f t="shared" si="12"/>
         <v>-7.0047926677872185E-2</v>
       </c>
-      <c r="U21" s="2">
+      <c r="U25" s="2">
         <v>2.074428769230769</v>
       </c>
-      <c r="V21" s="2">
+      <c r="V25" s="2">
         <v>1.6128481538461539</v>
       </c>
-      <c r="W21" s="2">
+      <c r="W25" s="2">
         <v>1.9873785569318201</v>
       </c>
-      <c r="X21" s="2">
+      <c r="X25" s="2">
         <v>2.9665530842886501</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="76" t="s">
+    <row r="26" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="40">
+        <v>5</v>
+      </c>
+      <c r="B26" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="41">
+        <v>8.5194595330739293</v>
+      </c>
+      <c r="D26" s="41">
+        <v>0.3111203682459977</v>
+      </c>
+      <c r="E26" s="43">
+        <f t="shared" si="0"/>
+        <v>3.6518791718908664E-2</v>
+      </c>
+      <c r="F26" s="42">
+        <f t="shared" ref="F26" si="63">$C$1+U26</f>
+        <v>7.9046312256634916</v>
+      </c>
+      <c r="G26" s="41">
+        <f t="shared" ref="G26" si="64">$C26-F26</f>
+        <v>0.6148283074104377</v>
+      </c>
+      <c r="H26" s="43">
+        <f t="shared" ref="H26" si="65">1-F26/$C26</f>
+        <v>7.2167524832247198E-2</v>
+      </c>
+      <c r="I26" s="42">
+        <f t="shared" ref="I26" si="66">$C$1+V26</f>
+        <v>7.2769852962052211</v>
+      </c>
+      <c r="J26" s="41">
+        <f t="shared" ref="J26" si="67">$C26-I26</f>
+        <v>1.2424742368687083</v>
+      </c>
+      <c r="K26" s="43">
+        <f t="shared" ref="K26" si="68">1-I26/$C26</f>
+        <v>0.14583956083660243</v>
+      </c>
+      <c r="L26" s="42">
+        <f t="shared" ref="L26" si="69">$C$1+W26</f>
+        <v>7.6493222801148413</v>
+      </c>
+      <c r="M26" s="41">
+        <f t="shared" ref="M26" si="70">$C26-L26</f>
+        <v>0.87013725295908806</v>
+      </c>
+      <c r="N26" s="43">
+        <f t="shared" ref="N26" si="71">1-L26/$C26</f>
+        <v>0.10213526451778698</v>
+      </c>
+      <c r="O26" s="41">
+        <f t="shared" ref="O26" si="72">$C$1+X26</f>
+        <v>8.7058591417414206</v>
+      </c>
+      <c r="P26" s="41">
+        <f t="shared" ref="P26" si="73">$C26-O26</f>
+        <v>-0.18639960866749128</v>
+      </c>
+      <c r="Q26" s="44">
+        <f t="shared" ref="Q26" si="74">1-O26/$C26</f>
+        <v>-2.1879276255008628E-2</v>
+      </c>
+      <c r="U26" s="2">
+        <v>2.2086245448428801</v>
+      </c>
+      <c r="V26" s="2">
+        <v>1.5809786153846099</v>
+      </c>
+      <c r="W26" s="2">
+        <v>1.9533155992942299</v>
+      </c>
+      <c r="X26" s="2">
+        <v>3.0098524609208099</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="77"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="57">
-        <f>AVERAGE(G7:G21)</f>
-        <v>9.5650499138653977E-2</v>
-      </c>
-      <c r="H22" s="60">
-        <f>AVERAGE(H7:H21)</f>
-        <v>1.0406349392129765E-2</v>
-      </c>
-      <c r="I22" s="59"/>
-      <c r="J22" s="57">
-        <f>AVERAGE(J7:J21)</f>
-        <v>0.64251723332668809</v>
-      </c>
-      <c r="K22" s="60">
-        <f>AVERAGE(K7:K21)</f>
-        <v>7.7797052324587612E-2</v>
-      </c>
-      <c r="L22" s="59"/>
-      <c r="M22" s="57">
-        <f>AVERAGE(M7:M21)</f>
-        <v>0.25237704279213025</v>
-      </c>
-      <c r="N22" s="60">
-        <f>AVERAGE(N7:N21)</f>
-        <v>2.9623969112347371E-2</v>
-      </c>
-      <c r="O22" s="57"/>
-      <c r="P22" s="57">
-        <f>AVERAGE(P7:P21)</f>
-        <v>-0.5647119529064677</v>
-      </c>
-      <c r="Q22" s="61">
-        <f>AVERAGE(Q7:Q21)</f>
-        <v>-7.2035855127415074E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="82" t="s">
+      <c r="B27" s="77"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="57">
+        <f>AVERAGE(G7:G25)</f>
+        <v>0.11744899319104732</v>
+      </c>
+      <c r="H27" s="60">
+        <f>AVERAGE(H7:H25)</f>
+        <v>1.3460577421533866E-2</v>
+      </c>
+      <c r="I27" s="59"/>
+      <c r="J27" s="57">
+        <f>AVERAGE(J7:J25)</f>
+        <v>0.67038911332116324</v>
+      </c>
+      <c r="K27" s="60">
+        <f>AVERAGE(K7:K25)</f>
+        <v>8.1903771015631663E-2</v>
+      </c>
+      <c r="L27" s="59"/>
+      <c r="M27" s="57">
+        <f>AVERAGE(M7:M25)</f>
+        <v>0.28263794645359708</v>
+      </c>
+      <c r="N27" s="60">
+        <f>AVERAGE(N7:N25)</f>
+        <v>3.3841561162063105E-2</v>
+      </c>
+      <c r="O27" s="57"/>
+      <c r="P27" s="57">
+        <f>AVERAGE(P7:P25)</f>
+        <v>-0.58786108079224186</v>
+      </c>
+      <c r="Q27" s="61">
+        <f>AVERAGE(Q7:Q25)</f>
+        <v>-7.4761550023384332E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="83"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="57">
-        <f>_xlfn.STDEV.P(G7:G21)</f>
-        <v>0.27951700210040503</v>
-      </c>
-      <c r="H23" s="60">
-        <f>_xlfn.STDEV.P(H7:H21)</f>
-        <v>3.4850699362246405E-2</v>
-      </c>
-      <c r="I23" s="59"/>
-      <c r="J23" s="57">
-        <f>_xlfn.STDEV.P(J7:J21)</f>
-        <v>0.28518734516629562</v>
-      </c>
-      <c r="K23" s="60">
-        <f>_xlfn.STDEV.P(K7:K21)</f>
-        <v>3.2956195486310701E-2</v>
-      </c>
-      <c r="L23" s="59"/>
-      <c r="M23" s="57">
-        <f>_xlfn.STDEV.P(M7:M21)</f>
-        <v>0.26205657748925093</v>
-      </c>
-      <c r="N23" s="60">
-        <f>_xlfn.STDEV.P(N7:N21)</f>
-        <v>3.1480880879445935E-2</v>
-      </c>
-      <c r="O23" s="57"/>
-      <c r="P23" s="57">
-        <f>_xlfn.STDEV.P(P7:P21)</f>
-        <v>0.42147520272715733</v>
-      </c>
-      <c r="Q23" s="61">
-        <f>_xlfn.STDEV.P(Q7:Q21)</f>
-        <v>5.3797735305745928E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A24" s="78" t="s">
+      <c r="B28" s="77"/>
+      <c r="C28" s="57"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="57">
+        <f>_xlfn.STDEV.P(G7:G25)</f>
+        <v>0.25449072716013937</v>
+      </c>
+      <c r="H28" s="60">
+        <f>_xlfn.STDEV.P(H7:H25)</f>
+        <v>3.1813705182117256E-2</v>
+      </c>
+      <c r="I28" s="59"/>
+      <c r="J28" s="57">
+        <f>_xlfn.STDEV.P(J7:J25)</f>
+        <v>0.27049455124562205</v>
+      </c>
+      <c r="K28" s="60">
+        <f>_xlfn.STDEV.P(K7:K25)</f>
+        <v>3.1558074918878493E-2</v>
+      </c>
+      <c r="L28" s="59"/>
+      <c r="M28" s="57">
+        <f>_xlfn.STDEV.P(M7:M25)</f>
+        <v>0.24631582589979345</v>
+      </c>
+      <c r="N28" s="60">
+        <f>_xlfn.STDEV.P(N7:N25)</f>
+        <v>2.9836520956183131E-2</v>
+      </c>
+      <c r="O28" s="57"/>
+      <c r="P28" s="57">
+        <f>_xlfn.STDEV.P(P7:P25)</f>
+        <v>0.38027469914384182</v>
+      </c>
+      <c r="Q28" s="61">
+        <f>_xlfn.STDEV.P(Q7:Q25)</f>
+        <v>4.8419861144512057E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A29" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="79"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="5" cm="1">
-        <f t="array" ref="G24">AVERAGE(ABS(G7:G21))</f>
-        <v>0.24917973811656235</v>
-      </c>
-      <c r="H24" s="11" cm="1">
-        <f t="array" ref="H24">AVERAGE(ABS(H7:H21))</f>
-        <v>3.0608340374776184E-2</v>
-      </c>
-      <c r="I24" s="12"/>
-      <c r="J24" s="5" cm="1">
-        <f t="array" ref="J24">AVERAGE(ABS(J7:J21))</f>
-        <v>0.64251723332668809</v>
-      </c>
-      <c r="K24" s="11" cm="1">
-        <f t="array" ref="K24">AVERAGE(ABS(K7:K21))</f>
-        <v>7.7797052324587612E-2</v>
-      </c>
-      <c r="L24" s="12"/>
-      <c r="M24" s="5" cm="1">
-        <f t="array" ref="M24">AVERAGE(ABS(M7:M21))</f>
-        <v>0.305333972212053</v>
-      </c>
-      <c r="N24" s="11" cm="1">
-        <f t="array" ref="N24">AVERAGE(ABS(N7:N21))</f>
-        <v>3.6824179548137652E-2</v>
-      </c>
-      <c r="O24" s="4"/>
-      <c r="P24" s="5" cm="1">
-        <f t="array" ref="P24">AVERAGE(ABS(P7:P21))</f>
-        <v>0.62136485478786874</v>
-      </c>
-      <c r="Q24" s="6" cm="1">
-        <f t="array" ref="Q24">AVERAGE(ABS(Q7:Q21))</f>
-        <v>7.8437469903460261E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A25" s="78" t="s">
+      <c r="B29" s="79"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="5" cm="1">
+        <f t="array" ref="G29">AVERAGE(ABS(G7:G25))</f>
+        <v>0.23865628712097497</v>
+      </c>
+      <c r="H29" s="11" cm="1">
+        <f t="array" ref="H29">AVERAGE(ABS(H7:H25))</f>
+        <v>2.9409517670991564E-2</v>
+      </c>
+      <c r="I29" s="12"/>
+      <c r="J29" s="5" cm="1">
+        <f t="array" ref="J29">AVERAGE(ABS(J7:J25))</f>
+        <v>0.67038911332116324</v>
+      </c>
+      <c r="K29" s="11" cm="1">
+        <f t="array" ref="K29">AVERAGE(ABS(K7:K25))</f>
+        <v>8.1903771015631663E-2</v>
+      </c>
+      <c r="L29" s="12"/>
+      <c r="M29" s="5" cm="1">
+        <f t="array" ref="M29">AVERAGE(ABS(M7:M25))</f>
+        <v>0.32444604862722026</v>
+      </c>
+      <c r="N29" s="11" cm="1">
+        <f t="array" ref="N29">AVERAGE(ABS(N7:N25))</f>
+        <v>3.9525937821897533E-2</v>
+      </c>
+      <c r="O29" s="4"/>
+      <c r="P29" s="5" cm="1">
+        <f t="array" ref="P29">AVERAGE(ABS(P7:P25))</f>
+        <v>0.6325870559617689</v>
+      </c>
+      <c r="Q29" s="6" cm="1">
+        <f t="array" ref="Q29">AVERAGE(ABS(Q7:Q25))</f>
+        <v>7.9815456425525289E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A30" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="79"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="5" cm="1">
-        <f t="array" ref="G25">_xlfn.STDEV.P(ABS(G7:G21))</f>
-        <v>0.15870800408559391</v>
-      </c>
-      <c r="H25" s="11" cm="1">
-        <f t="array" ref="H25">_xlfn.STDEV.P(ABS(H7:H21))</f>
-        <v>1.9646700822545427E-2</v>
-      </c>
-      <c r="I25" s="12"/>
-      <c r="J25" s="5" cm="1">
-        <f t="array" ref="J25">_xlfn.STDEV.P(ABS(J7:J21))</f>
-        <v>0.28518734516629562</v>
-      </c>
-      <c r="K25" s="11" cm="1">
-        <f t="array" ref="K25">_xlfn.STDEV.P(ABS(K7:K21))</f>
-        <v>3.2956195486310701E-2</v>
-      </c>
-      <c r="L25" s="12"/>
-      <c r="M25" s="5" cm="1">
-        <f t="array" ref="M25">_xlfn.STDEV.P(ABS(M7:M21))</f>
-        <v>0.19783575750376825</v>
-      </c>
-      <c r="N25" s="11" cm="1">
-        <f t="array" ref="N25">_xlfn.STDEV.P(ABS(N7:N21))</f>
-        <v>2.2640786371539674E-2</v>
-      </c>
-      <c r="O25" s="4"/>
-      <c r="P25" s="5" cm="1">
-        <f t="array" ref="P25">_xlfn.STDEV.P(ABS(P7:P21))</f>
-        <v>0.3323351523745055</v>
-      </c>
-      <c r="Q25" s="6" cm="1">
-        <f t="array" ref="Q25">_xlfn.STDEV.P(ABS(Q7:Q21))</f>
-        <v>4.3942281041256824E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A26" s="78" t="s">
+      <c r="B30" s="79"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="5" cm="1">
+        <f t="array" ref="G30">_xlfn.STDEV.P(ABS(G7:G25))</f>
+        <v>0.14697949799110735</v>
+      </c>
+      <c r="H30" s="11" cm="1">
+        <f t="array" ref="H30">_xlfn.STDEV.P(ABS(H7:H25))</f>
+        <v>1.8121237603856331E-2</v>
+      </c>
+      <c r="I30" s="12"/>
+      <c r="J30" s="5" cm="1">
+        <f t="array" ref="J30">_xlfn.STDEV.P(ABS(J7:J25))</f>
+        <v>0.27049455124562205</v>
+      </c>
+      <c r="K30" s="11" cm="1">
+        <f t="array" ref="K30">_xlfn.STDEV.P(ABS(K7:K25))</f>
+        <v>3.1558074918878493E-2</v>
+      </c>
+      <c r="L30" s="12"/>
+      <c r="M30" s="5" cm="1">
+        <f t="array" ref="M30">_xlfn.STDEV.P(ABS(M7:M25))</f>
+        <v>0.18785754282005071</v>
+      </c>
+      <c r="N30" s="11" cm="1">
+        <f t="array" ref="N30">_xlfn.STDEV.P(ABS(N7:N25))</f>
+        <v>2.1752459262205339E-2</v>
+      </c>
+      <c r="O30" s="4"/>
+      <c r="P30" s="5" cm="1">
+        <f t="array" ref="P30">_xlfn.STDEV.P(ABS(P7:P25))</f>
+        <v>0.30003852044159923</v>
+      </c>
+      <c r="Q30" s="6" cm="1">
+        <f t="array" ref="Q30">_xlfn.STDEV.P(ABS(Q7:Q25))</f>
+        <v>3.9538149055537493E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A31" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="79"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="5" cm="1">
-        <f t="array" ref="G26">MAX(ABS(G7:G21))</f>
+      <c r="B31" s="79"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="5" cm="1">
+        <f t="array" ref="G31">MAX(ABS(G7:G25))</f>
         <v>0.56371083519219667</v>
       </c>
-      <c r="H26" s="11" cm="1">
-        <f t="array" ref="H26">MAX(ABS(H7:H21))</f>
+      <c r="H31" s="11" cm="1">
+        <f t="array" ref="H31">MAX(ABS(H7:H25))</f>
         <v>7.5533209795243472E-2</v>
       </c>
-      <c r="I26" s="12"/>
-      <c r="J26" s="5" cm="1">
-        <f t="array" ref="J26">MAX(ABS(J7:J21))</f>
+      <c r="I31" s="12"/>
+      <c r="J31" s="5" cm="1">
+        <f t="array" ref="J31">MAX(ABS(J7:J25))</f>
         <v>1.0261441482392168</v>
       </c>
-      <c r="K26" s="11" cm="1">
-        <f t="array" ref="K26">MAX(ABS(K7:K21))</f>
-        <v>0.11653453500106425</v>
-      </c>
-      <c r="L26" s="12"/>
-      <c r="M26" s="5" cm="1">
-        <f t="array" ref="M26">MAX(ABS(M7:M21))</f>
+      <c r="K31" s="11" cm="1">
+        <f t="array" ref="K31">MAX(ABS(K7:K25))</f>
+        <v>0.11758006071550631</v>
+      </c>
+      <c r="L31" s="12"/>
+      <c r="M31" s="5" cm="1">
+        <f t="array" ref="M31">MAX(ABS(M7:M25))</f>
         <v>0.7058442317682232</v>
       </c>
-      <c r="N26" s="11" cm="1">
-        <f t="array" ref="N26">MAX(ABS(N7:N21))</f>
+      <c r="N31" s="11" cm="1">
+        <f t="array" ref="N31">MAX(ABS(N7:N25))</f>
         <v>7.9107847191901115E-2</v>
       </c>
-      <c r="O26" s="4"/>
-      <c r="P26" s="5" cm="1">
-        <f t="array" ref="P26">MAX(ABS(P7:P21))</f>
+      <c r="O31" s="4"/>
+      <c r="P31" s="5" cm="1">
+        <f t="array" ref="P31">MAX(ABS(P7:P25))</f>
         <v>1.1378227070112636</v>
       </c>
-      <c r="Q26" s="6" cm="1">
-        <f t="array" ref="Q26">MAX(ABS(Q7:Q21))</f>
+      <c r="Q31" s="6" cm="1">
+        <f t="array" ref="Q31">MAX(ABS(Q7:Q25))</f>
         <v>0.13877515790397443</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="80" t="s">
+    <row r="32" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="81"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="1" cm="1">
-        <f t="array" ref="G27">MIN(ABS(G7:G21))</f>
+      <c r="B32" s="81"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="1" cm="1">
+        <f t="array" ref="G32">MIN(ABS(G7:G25))</f>
         <v>1.4130608936810063E-2</v>
       </c>
-      <c r="H27" s="14" cm="1">
-        <f t="array" ref="H27">MIN(ABS(H7:H21))</f>
+      <c r="H32" s="14" cm="1">
+        <f t="array" ref="H32">MIN(ABS(H7:H25))</f>
         <v>1.7234473124869698E-3</v>
       </c>
-      <c r="I27" s="13"/>
-      <c r="J27" s="1" cm="1">
-        <f t="array" ref="J27">MIN(ABS(J7:J21))</f>
+      <c r="I32" s="13"/>
+      <c r="J32" s="1" cm="1">
+        <f t="array" ref="J32">MIN(ABS(J7:J25))</f>
         <v>0.16327629845039571</v>
       </c>
-      <c r="K27" s="14" cm="1">
-        <f t="array" ref="K27">MIN(ABS(K7:K21))</f>
+      <c r="K32" s="14" cm="1">
+        <f t="array" ref="K32">MIN(ABS(K7:K25))</f>
         <v>2.2563181005000876E-2</v>
       </c>
-      <c r="L27" s="13"/>
-      <c r="M27" s="1" cm="1">
-        <f t="array" ref="M27">MIN(ABS(M7:M21))</f>
+      <c r="L32" s="13"/>
+      <c r="M32" s="1" cm="1">
+        <f t="array" ref="M32">MIN(ABS(M7:M25))</f>
         <v>1.8250825119585201E-2</v>
       </c>
-      <c r="N27" s="14" cm="1">
-        <f t="array" ref="N27">MIN(ABS(N7:N21))</f>
+      <c r="N32" s="14" cm="1">
+        <f t="array" ref="N32">MIN(ABS(N7:N25))</f>
         <v>2.240271085906409E-3</v>
       </c>
-      <c r="O27" s="7"/>
-      <c r="P27" s="1" cm="1">
-        <f t="array" ref="P27">MIN(ABS(P7:P21))</f>
+      <c r="O32" s="7"/>
+      <c r="P32" s="1" cm="1">
+        <f t="array" ref="P32">MIN(ABS(P7:P25))</f>
         <v>2.8329665201379584E-2</v>
       </c>
-      <c r="Q27" s="8" cm="1">
-        <f t="array" ref="Q27">MIN(ABS(Q7:Q21))</f>
+      <c r="Q32" s="8" cm="1">
+        <f t="array" ref="Q32">MIN(ABS(Q7:Q25))</f>
         <v>3.150812184177898E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="35" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q30"/>
-    </row>
-    <row r="32" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="K32"/>
-    </row>
-    <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="J33"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="Q35"/>
+    </row>
+    <row r="37" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="K37"/>
+    </row>
+    <row r="38" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="J38"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="G35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+    <row r="40" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="G40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="I5:K5"/>

</xml_diff>

<commit_message>
fixed issues with experiment 6 predictor comparison table
</commit_message>
<xml_diff>
--- a/experiments/09_power_eval_1/predictor_comp.xlsx
+++ b/experiments/09_power_eval_1/predictor_comp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_TEMP2\experiment_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FEC553-EDFB-4974-A431-ADB95A167A93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCE99A9-D1B1-42A4-89D0-86A54E8B95C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{39932099-E81A-42DA-B46C-E67CD6F446DD}"/>
   </bookViews>
@@ -578,13 +578,30 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -626,23 +643,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1211,7 +1213,7 @@
   <dimension ref="A1:X47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1232,76 +1234,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="64"/>
+      <c r="B1" s="69"/>
       <c r="C1" s="55">
         <v>5.6960066808206111</v>
       </c>
-      <c r="D1" s="55"/>
-      <c r="E1" s="56" t="s">
+      <c r="D1" s="81" t="s">
         <v>2</v>
       </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="3" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="74" t="s">
+      <c r="C4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="74"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="74" t="s">
+      <c r="D4" s="79"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="74"/>
-      <c r="Q4" s="75"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="79"/>
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="80"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="70"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="65" t="s">
+      <c r="A5" s="75"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="66"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="65" t="s">
+      <c r="G5" s="71"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="66"/>
-      <c r="K5" s="67"/>
-      <c r="L5" s="65" t="s">
+      <c r="J5" s="71"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="66"/>
-      <c r="N5" s="67"/>
-      <c r="O5" s="66" t="s">
+      <c r="M5" s="71"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="68"/>
+      <c r="P5" s="71"/>
+      <c r="Q5" s="73"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="71"/>
-      <c r="B6" s="73"/>
+      <c r="A6" s="76"/>
+      <c r="B6" s="78"/>
       <c r="C6" s="45" t="s">
         <v>4</v>
       </c>
@@ -1344,7 +1347,7 @@
       <c r="P6" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="Q6" s="62" t="s">
+      <c r="Q6" s="61" t="s">
         <v>11</v>
       </c>
       <c r="U6" s="2" t="s">
@@ -2921,272 +2924,272 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="76" t="s">
+      <c r="A27" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="77"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="57">
-        <f>AVERAGE(G7:G25)</f>
-        <v>0.11744899319104732</v>
-      </c>
-      <c r="H27" s="60">
-        <f>AVERAGE(H7:H25)</f>
-        <v>1.3460577421533866E-2</v>
-      </c>
-      <c r="I27" s="59"/>
-      <c r="J27" s="57">
-        <f>AVERAGE(J7:J25)</f>
-        <v>0.67038911332116324</v>
-      </c>
-      <c r="K27" s="60">
-        <f>AVERAGE(K7:K25)</f>
-        <v>8.1903771015631663E-2</v>
-      </c>
-      <c r="L27" s="59"/>
-      <c r="M27" s="57">
-        <f>AVERAGE(M7:M25)</f>
-        <v>0.28263794645359708</v>
-      </c>
-      <c r="N27" s="60">
-        <f>AVERAGE(N7:N25)</f>
-        <v>3.3841561162063105E-2</v>
-      </c>
-      <c r="O27" s="57"/>
-      <c r="P27" s="57">
-        <f>AVERAGE(P7:P25)</f>
-        <v>-0.58786108079224186</v>
-      </c>
-      <c r="Q27" s="61">
-        <f>AVERAGE(Q7:Q25)</f>
-        <v>-7.4761550023384332E-2</v>
+      <c r="B27" s="63"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="56">
+        <f>AVERAGE(G7:G26)</f>
+        <v>0.14231795890201684</v>
+      </c>
+      <c r="H27" s="59">
+        <f>AVERAGE(H7:H26)</f>
+        <v>1.6395924792069534E-2</v>
+      </c>
+      <c r="I27" s="58"/>
+      <c r="J27" s="56">
+        <f>AVERAGE(J7:J26)</f>
+        <v>0.69899336949854052</v>
+      </c>
+      <c r="K27" s="59">
+        <f>AVERAGE(K7:K26)</f>
+        <v>8.5100560506680203E-2</v>
+      </c>
+      <c r="L27" s="58"/>
+      <c r="M27" s="56">
+        <f>AVERAGE(M7:M26)</f>
+        <v>0.31201291177887158</v>
+      </c>
+      <c r="N27" s="59">
+        <f>AVERAGE(N7:N26)</f>
+        <v>3.7256246329849294E-2</v>
+      </c>
+      <c r="O27" s="56"/>
+      <c r="P27" s="56">
+        <f>AVERAGE(P7:P26)</f>
+        <v>-0.56778800718600431</v>
+      </c>
+      <c r="Q27" s="60">
+        <f>AVERAGE(Q7:Q26)</f>
+        <v>-7.2117436334965548E-2</v>
       </c>
     </row>
     <row r="28" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="76" t="s">
+      <c r="A28" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="77"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="57">
-        <f>_xlfn.STDEV.P(G7:G25)</f>
-        <v>0.25449072716013937</v>
-      </c>
-      <c r="H28" s="60">
-        <f>_xlfn.STDEV.P(H7:H25)</f>
-        <v>3.1813705182117256E-2</v>
-      </c>
-      <c r="I28" s="59"/>
-      <c r="J28" s="57">
-        <f>_xlfn.STDEV.P(J7:J25)</f>
-        <v>0.27049455124562205</v>
-      </c>
-      <c r="K28" s="60">
-        <f>_xlfn.STDEV.P(K7:K25)</f>
-        <v>3.1558074918878493E-2</v>
-      </c>
-      <c r="L28" s="59"/>
-      <c r="M28" s="57">
-        <f>_xlfn.STDEV.P(M7:M25)</f>
-        <v>0.24631582589979345</v>
-      </c>
-      <c r="N28" s="60">
-        <f>_xlfn.STDEV.P(N7:N25)</f>
-        <v>2.9836520956183131E-2</v>
-      </c>
-      <c r="O28" s="57"/>
-      <c r="P28" s="57">
-        <f>_xlfn.STDEV.P(P7:P25)</f>
-        <v>0.38027469914384182</v>
-      </c>
-      <c r="Q28" s="61">
-        <f>_xlfn.STDEV.P(Q7:Q25)</f>
-        <v>4.8419861144512057E-2</v>
+      <c r="B28" s="63"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="56">
+        <f>_xlfn.STDEV.P(G7:G26)</f>
+        <v>0.27069927475910577</v>
+      </c>
+      <c r="H28" s="59">
+        <f>_xlfn.STDEV.P(H7:H26)</f>
+        <v>3.3544228491238892E-2</v>
+      </c>
+      <c r="I28" s="58"/>
+      <c r="J28" s="56">
+        <f>_xlfn.STDEV.P(J7:J26)</f>
+        <v>0.29164156613667291</v>
+      </c>
+      <c r="K28" s="59">
+        <f>_xlfn.STDEV.P(K7:K26)</f>
+        <v>3.3768125294540104E-2</v>
+      </c>
+      <c r="L28" s="58"/>
+      <c r="M28" s="56">
+        <f>_xlfn.STDEV.P(M7:M26)</f>
+        <v>0.27208968182131243</v>
+      </c>
+      <c r="N28" s="59">
+        <f>_xlfn.STDEV.P(N7:N26)</f>
+        <v>3.2668769562644979E-2</v>
+      </c>
+      <c r="O28" s="56"/>
+      <c r="P28" s="56">
+        <f>_xlfn.STDEV.P(P7:P26)</f>
+        <v>0.38083335182796119</v>
+      </c>
+      <c r="Q28" s="60">
+        <f>_xlfn.STDEV.P(Q7:Q26)</f>
+        <v>4.8580800861446546E-2</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A29" s="78" t="s">
+      <c r="A29" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="79"/>
+      <c r="B29" s="65"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="9"/>
       <c r="F29" s="12"/>
       <c r="G29" s="5" cm="1">
-        <f t="array" ref="G29">AVERAGE(ABS(G7:G25))</f>
-        <v>0.23865628712097497</v>
+        <f t="array" ref="G29">AVERAGE(ABS(G7:G26))</f>
+        <v>0.2574648881354481</v>
       </c>
       <c r="H29" s="11" cm="1">
-        <f t="array" ref="H29">AVERAGE(ABS(H7:H25))</f>
-        <v>2.9409517670991564E-2</v>
+        <f t="array" ref="H29">AVERAGE(ABS(H7:H26))</f>
+        <v>3.154741802905435E-2</v>
       </c>
       <c r="I29" s="12"/>
       <c r="J29" s="5" cm="1">
-        <f t="array" ref="J29">AVERAGE(ABS(J7:J25))</f>
-        <v>0.67038911332116324</v>
+        <f t="array" ref="J29">AVERAGE(ABS(J7:J26))</f>
+        <v>0.69899336949854052</v>
       </c>
       <c r="K29" s="11" cm="1">
-        <f t="array" ref="K29">AVERAGE(ABS(K7:K25))</f>
-        <v>8.1903771015631663E-2</v>
+        <f t="array" ref="K29">AVERAGE(ABS(K7:K26))</f>
+        <v>8.5100560506680203E-2</v>
       </c>
       <c r="L29" s="12"/>
       <c r="M29" s="5" cm="1">
-        <f t="array" ref="M29">AVERAGE(ABS(M7:M25))</f>
-        <v>0.32444604862722026</v>
+        <f t="array" ref="M29">AVERAGE(ABS(M7:M26))</f>
+        <v>0.35173060884381363</v>
       </c>
       <c r="N29" s="11" cm="1">
-        <f t="array" ref="N29">AVERAGE(ABS(N7:N25))</f>
-        <v>3.9525937821897533E-2</v>
+        <f t="array" ref="N29">AVERAGE(ABS(N7:N26))</f>
+        <v>4.2656404156692009E-2</v>
       </c>
       <c r="O29" s="4"/>
       <c r="P29" s="5" cm="1">
-        <f t="array" ref="P29">AVERAGE(ABS(P7:P25))</f>
-        <v>0.6325870559617689</v>
+        <f t="array" ref="P29">AVERAGE(ABS(P7:P26))</f>
+        <v>0.61027768359705503</v>
       </c>
       <c r="Q29" s="6" cm="1">
-        <f t="array" ref="Q29">AVERAGE(ABS(Q7:Q25))</f>
-        <v>7.9815456425525289E-2</v>
+        <f t="array" ref="Q29">AVERAGE(ABS(Q7:Q26))</f>
+        <v>7.6918647416999456E-2</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A30" s="78" t="s">
+      <c r="A30" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="79"/>
+      <c r="B30" s="65"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="9"/>
       <c r="F30" s="12"/>
       <c r="G30" s="5" cm="1">
-        <f t="array" ref="G30">_xlfn.STDEV.P(ABS(G7:G25))</f>
-        <v>0.14697949799110735</v>
+        <f t="array" ref="G30">_xlfn.STDEV.P(ABS(G7:G26))</f>
+        <v>0.1650585658441972</v>
       </c>
       <c r="H30" s="11" cm="1">
-        <f t="array" ref="H30">_xlfn.STDEV.P(ABS(H7:H25))</f>
-        <v>1.8121237603856331E-2</v>
+        <f t="array" ref="H30">_xlfn.STDEV.P(ABS(H7:H26))</f>
+        <v>1.9970028306433123E-2</v>
       </c>
       <c r="I30" s="12"/>
       <c r="J30" s="5" cm="1">
-        <f t="array" ref="J30">_xlfn.STDEV.P(ABS(J7:J25))</f>
-        <v>0.27049455124562205</v>
+        <f t="array" ref="J30">_xlfn.STDEV.P(ABS(J7:J26))</f>
+        <v>0.29164156613667291</v>
       </c>
       <c r="K30" s="11" cm="1">
-        <f t="array" ref="K30">_xlfn.STDEV.P(ABS(K7:K25))</f>
-        <v>3.1558074918878493E-2</v>
+        <f t="array" ref="K30">_xlfn.STDEV.P(ABS(K7:K26))</f>
+        <v>3.3768125294540104E-2</v>
       </c>
       <c r="L30" s="12"/>
       <c r="M30" s="5" cm="1">
-        <f t="array" ref="M30">_xlfn.STDEV.P(ABS(M7:M25))</f>
-        <v>0.18785754282005071</v>
+        <f t="array" ref="M30">_xlfn.STDEV.P(ABS(M7:M26))</f>
+        <v>0.21833559231768215</v>
       </c>
       <c r="N30" s="11" cm="1">
-        <f t="array" ref="N30">_xlfn.STDEV.P(ABS(N7:N25))</f>
-        <v>2.1752459262205339E-2</v>
+        <f t="array" ref="N30">_xlfn.STDEV.P(ABS(N7:N26))</f>
+        <v>2.521324215067465E-2</v>
       </c>
       <c r="O30" s="4"/>
       <c r="P30" s="5" cm="1">
-        <f t="array" ref="P30">_xlfn.STDEV.P(ABS(P7:P25))</f>
-        <v>0.30003852044159923</v>
+        <f t="array" ref="P30">_xlfn.STDEV.P(ABS(P7:P26))</f>
+        <v>0.30818567759093957</v>
       </c>
       <c r="Q30" s="6" cm="1">
-        <f t="array" ref="Q30">_xlfn.STDEV.P(ABS(Q7:Q25))</f>
-        <v>3.9538149055537493E-2</v>
+        <f t="array" ref="Q30">_xlfn.STDEV.P(ABS(Q7:Q26))</f>
+        <v>4.0552934732355161E-2</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A31" s="78" t="s">
+      <c r="A31" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="79"/>
+      <c r="B31" s="65"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="9"/>
       <c r="F31" s="12"/>
       <c r="G31" s="5" cm="1">
-        <f t="array" ref="G31">MAX(ABS(G7:G25))</f>
-        <v>0.56371083519219667</v>
+        <f t="array" ref="G31">MAX(ABS(G7:G26))</f>
+        <v>0.6148283074104377</v>
       </c>
       <c r="H31" s="11" cm="1">
-        <f t="array" ref="H31">MAX(ABS(H7:H25))</f>
+        <f t="array" ref="H31">MAX(ABS(H7:H26))</f>
         <v>7.5533209795243472E-2</v>
       </c>
       <c r="I31" s="12"/>
       <c r="J31" s="5" cm="1">
-        <f t="array" ref="J31">MAX(ABS(J7:J25))</f>
-        <v>1.0261441482392168</v>
+        <f t="array" ref="J31">MAX(ABS(J7:J26))</f>
+        <v>1.2424742368687083</v>
       </c>
       <c r="K31" s="11" cm="1">
-        <f t="array" ref="K31">MAX(ABS(K7:K25))</f>
-        <v>0.11758006071550631</v>
+        <f t="array" ref="K31">MAX(ABS(K7:K26))</f>
+        <v>0.14583956083660243</v>
       </c>
       <c r="L31" s="12"/>
       <c r="M31" s="5" cm="1">
-        <f t="array" ref="M31">MAX(ABS(M7:M25))</f>
-        <v>0.7058442317682232</v>
+        <f t="array" ref="M31">MAX(ABS(M7:M26))</f>
+        <v>0.87013725295908806</v>
       </c>
       <c r="N31" s="11" cm="1">
-        <f t="array" ref="N31">MAX(ABS(N7:N25))</f>
-        <v>7.9107847191901115E-2</v>
+        <f t="array" ref="N31">MAX(ABS(N7:N26))</f>
+        <v>0.10213526451778698</v>
       </c>
       <c r="O31" s="4"/>
       <c r="P31" s="5" cm="1">
-        <f t="array" ref="P31">MAX(ABS(P7:P25))</f>
+        <f t="array" ref="P31">MAX(ABS(P7:P26))</f>
         <v>1.1378227070112636</v>
       </c>
       <c r="Q31" s="6" cm="1">
-        <f t="array" ref="Q31">MAX(ABS(Q7:Q25))</f>
+        <f t="array" ref="Q31">MAX(ABS(Q7:Q26))</f>
         <v>0.13877515790397443</v>
       </c>
     </row>
     <row r="32" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="80" t="s">
+      <c r="A32" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="81"/>
+      <c r="B32" s="67"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="10"/>
       <c r="F32" s="13"/>
       <c r="G32" s="1" cm="1">
-        <f t="array" ref="G32">MIN(ABS(G7:G25))</f>
+        <f t="array" ref="G32">MIN(ABS(G7:G26))</f>
         <v>1.4130608936810063E-2</v>
       </c>
       <c r="H32" s="14" cm="1">
-        <f t="array" ref="H32">MIN(ABS(H7:H25))</f>
+        <f t="array" ref="H32">MIN(ABS(H7:H26))</f>
         <v>1.7234473124869698E-3</v>
       </c>
       <c r="I32" s="13"/>
       <c r="J32" s="1" cm="1">
-        <f t="array" ref="J32">MIN(ABS(J7:J25))</f>
+        <f t="array" ref="J32">MIN(ABS(J7:J26))</f>
         <v>0.16327629845039571</v>
       </c>
       <c r="K32" s="14" cm="1">
-        <f t="array" ref="K32">MIN(ABS(K7:K25))</f>
+        <f t="array" ref="K32">MIN(ABS(K7:K26))</f>
         <v>2.2563181005000876E-2</v>
       </c>
       <c r="L32" s="13"/>
       <c r="M32" s="1" cm="1">
-        <f t="array" ref="M32">MIN(ABS(M7:M25))</f>
+        <f t="array" ref="M32">MIN(ABS(M7:M26))</f>
         <v>1.8250825119585201E-2</v>
       </c>
       <c r="N32" s="14" cm="1">
-        <f t="array" ref="N32">MIN(ABS(N7:N25))</f>
+        <f t="array" ref="N32">MIN(ABS(N7:N26))</f>
         <v>2.240271085906409E-3</v>
       </c>
       <c r="O32" s="7"/>
       <c r="P32" s="1" cm="1">
-        <f t="array" ref="P32">MIN(ABS(P7:P25))</f>
+        <f t="array" ref="P32">MIN(ABS(P7:P26))</f>
         <v>2.8329665201379584E-2</v>
       </c>
       <c r="Q32" s="8" cm="1">
-        <f t="array" ref="Q32">MIN(ABS(Q7:Q25))</f>
+        <f t="array" ref="Q32">MIN(ABS(Q7:Q26))</f>
         <v>3.150812184177898E-3</v>
       </c>
     </row>
@@ -3224,12 +3227,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="I5:K5"/>
@@ -3239,6 +3236,12 @@
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:E5"/>
     <mergeCell ref="F4:Q4"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="61" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
corrected exp6 pred comp table
</commit_message>
<xml_diff>
--- a/experiments/09_power_eval_1/predictor_comp.xlsx
+++ b/experiments/09_power_eval_1/predictor_comp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_TEMP2\experiment_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDA191D-A0D2-4EA1-AD4A-CC7CBE0D52F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395CCC18-3FCF-4C21-B4B8-A1F02BF59930}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{39932099-E81A-42DA-B46C-E67CD6F446DD}"/>
   </bookViews>
@@ -315,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -408,17 +408,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -602,80 +591,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="6" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="6" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="6" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="6" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="6" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="6" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="6" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -684,37 +670,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -726,13 +694,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -740,6 +708,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1308,7 +1294,7 @@
   <dimension ref="A1:AB52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A32" sqref="A32:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1331,14 +1317,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="55">
+      <c r="B1" s="65"/>
+      <c r="C1" s="53">
         <v>5.6960066808206111</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="59" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="3"/>
@@ -1349,122 +1335,122 @@
     </row>
     <row r="3" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="84"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="84" t="s">
+      <c r="D4" s="75"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="84"/>
-      <c r="N4" s="84"/>
-      <c r="O4" s="84"/>
-      <c r="P4" s="84"/>
-      <c r="Q4" s="84"/>
-      <c r="R4" s="84"/>
-      <c r="S4" s="84"/>
-      <c r="T4" s="85"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="75"/>
+      <c r="M4" s="75"/>
+      <c r="N4" s="75"/>
+      <c r="O4" s="75"/>
+      <c r="P4" s="75"/>
+      <c r="Q4" s="75"/>
+      <c r="R4" s="75"/>
+      <c r="S4" s="75"/>
+      <c r="T4" s="76"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A5" s="80"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="75" t="s">
+      <c r="A5" s="71"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="76"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="75" t="s">
+      <c r="G5" s="67"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="76"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="75" t="s">
+      <c r="J5" s="67"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="76"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="75" t="s">
+      <c r="M5" s="67"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="76" t="s">
+      <c r="P5" s="67"/>
+      <c r="Q5" s="68"/>
+      <c r="R5" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="S5" s="76"/>
-      <c r="T5" s="78"/>
+      <c r="S5" s="67"/>
+      <c r="T5" s="69"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A6" s="81"/>
-      <c r="B6" s="83"/>
-      <c r="C6" s="45" t="s">
+      <c r="A6" s="72"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="45" t="s">
+      <c r="G6" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="48" t="s">
+      <c r="H6" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="45" t="s">
+      <c r="J6" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="48" t="s">
+      <c r="K6" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="47" t="s">
+      <c r="L6" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="45" t="s">
+      <c r="M6" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="46" t="s">
+      <c r="N6" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="47" t="s">
+      <c r="O6" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="45" t="s">
+      <c r="P6" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="Q6" s="46" t="s">
+      <c r="Q6" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="45" t="s">
+      <c r="R6" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="S6" s="45" t="s">
+      <c r="S6" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="T6" s="61" t="s">
+      <c r="T6" s="58" t="s">
         <v>11</v>
       </c>
       <c r="X6" s="2" t="s">
@@ -1484,79 +1470,79 @@
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A7" s="15">
+      <c r="A7" s="13">
         <v>1</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="14">
         <v>8.0554880581516084</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="14">
         <v>0.18071383312729691</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="16">
         <f>D7/C7</f>
         <v>2.2433629324846029E-2</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="15">
         <f>$C$1+X7</f>
         <v>7.8328429115898421</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="14">
         <f>$C7-F7</f>
         <v>0.22264514656176626</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="16">
         <f>1-F7/$C7</f>
         <v>2.7638939435390864E-2</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="15">
         <f>$C$1+Y7</f>
         <v>7.9143180143769314</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="14">
         <f>$C7-I7</f>
         <v>0.14117004377467701</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="16">
         <f>1-I7/$C7</f>
         <v>1.7524703997521596E-2</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="15">
         <f>$C$1+Z7</f>
         <v>7.2554734500513804</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="14">
         <f>$C7-L7</f>
         <v>0.80001460810022795</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="16">
         <f>1-L7/$C7</f>
         <v>9.9312990389287092E-2</v>
       </c>
-      <c r="O7" s="17">
+      <c r="O7" s="15">
         <f>$C$1+AA7</f>
         <v>7.6129914589675112</v>
       </c>
-      <c r="P7" s="16">
+      <c r="P7" s="14">
         <f>$C7-O7</f>
         <v>0.44249659918409723</v>
       </c>
-      <c r="Q7" s="18">
+      <c r="Q7" s="16">
         <f>1-O7/$C7</f>
         <v>5.4931072579310736E-2</v>
       </c>
-      <c r="R7" s="16">
+      <c r="R7" s="14">
         <f>$C$1+AB7</f>
         <v>8.4762292567487609</v>
       </c>
-      <c r="S7" s="16">
+      <c r="S7" s="14">
         <f>$C7-R7</f>
         <v>-0.42074119859715253</v>
       </c>
-      <c r="T7" s="19">
+      <c r="T7" s="17">
         <f>1-R7/$C7</f>
         <v>-5.2230379532546278E-2</v>
       </c>
@@ -1577,79 +1563,79 @@
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A8" s="15">
+      <c r="A8" s="13">
         <v>1</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="14">
         <v>8.6675039281705946</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="14">
         <v>0.18760700577356218</v>
       </c>
-      <c r="E8" s="18">
-        <f t="shared" ref="E8:E37" si="0">D8/C8</f>
+      <c r="E8" s="16">
+        <f t="shared" ref="E8:E31" si="0">D8/C8</f>
         <v>2.1644871156482927E-2</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="15">
         <f t="shared" ref="F8:F29" si="1">$C$1+X8</f>
         <v>8.3995216808206106</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="14">
         <f t="shared" ref="G8:G29" si="2">$C8-F8</f>
         <v>0.26798224734998399</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="16">
         <f t="shared" ref="H8:H29" si="3">1-F8/$C8</f>
         <v>3.0918041638147375E-2</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="15">
         <f t="shared" ref="I8:I31" si="4">$C$1+Y8</f>
         <v>8.4910786676157208</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="14">
         <f t="shared" ref="J8:J30" si="5">$C8-I8</f>
         <v>0.17642526055487373</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="16">
         <f t="shared" ref="K8:K30" si="6">1-I8/$C8</f>
         <v>2.0354794415664124E-2</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="15">
         <f t="shared" ref="L8:L29" si="7">$C$1+Z8</f>
         <v>8.0903201423590723</v>
       </c>
-      <c r="M8" s="16">
+      <c r="M8" s="14">
         <f t="shared" ref="M8:M29" si="8">$C8-L8</f>
         <v>0.5771837858115223</v>
       </c>
-      <c r="N8" s="18">
+      <c r="N8" s="16">
         <f t="shared" ref="N8:N29" si="9">1-L8/$C8</f>
         <v>6.6591695901699555E-2</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8" s="15">
         <f t="shared" ref="O8:O29" si="10">$C$1+AA8</f>
         <v>8.3022451476388515</v>
       </c>
-      <c r="P8" s="16">
+      <c r="P8" s="14">
         <f t="shared" ref="P8:P29" si="11">$C8-O8</f>
         <v>0.3652587805317431</v>
       </c>
-      <c r="Q8" s="18">
+      <c r="Q8" s="16">
         <f t="shared" ref="Q8:Q29" si="12">1-O8/$C8</f>
         <v>4.2141172771159807E-2</v>
       </c>
-      <c r="R8" s="16">
+      <c r="R8" s="14">
         <f t="shared" ref="R8:R29" si="13">$C$1+AB8</f>
         <v>8.548766422999341</v>
       </c>
-      <c r="S8" s="16">
+      <c r="S8" s="14">
         <f t="shared" ref="S8:S29" si="14">$C8-R8</f>
         <v>0.11873750517125359</v>
       </c>
-      <c r="T8" s="19">
+      <c r="T8" s="17">
         <f t="shared" ref="T8:T29" si="15">1-R8/$C8</f>
         <v>1.3699157930040284E-2</v>
       </c>
@@ -1670,79 +1656,79 @@
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A9" s="15">
+      <c r="A9" s="13">
         <v>1</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="14">
         <v>7.4526486486486485</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="14">
         <v>0.17484240700075782</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="16">
         <f t="shared" si="0"/>
         <v>2.346043873039166E-2</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="15">
         <f t="shared" si="1"/>
         <v>7.5647661423590726</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="14">
         <f t="shared" si="2"/>
         <v>-0.11211749371042412</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="16">
         <f t="shared" si="3"/>
         <v>-1.5043979529446139E-2</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="15">
         <f t="shared" si="4"/>
         <v>7.6235268541259913</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9" s="14">
         <f t="shared" si="5"/>
         <v>-0.17087820547734278</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="16">
         <f t="shared" si="6"/>
         <v>-2.2928520252773144E-2</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9" s="15">
         <f t="shared" si="7"/>
         <v>7.2269846038975345</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="14">
         <f t="shared" si="8"/>
         <v>0.22566404475111401</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N9" s="16">
         <f t="shared" si="9"/>
         <v>3.0279710662602155E-2</v>
       </c>
-      <c r="O9" s="17">
+      <c r="O9" s="15">
         <f t="shared" si="10"/>
         <v>7.5829813664253614</v>
       </c>
-      <c r="P9" s="16">
+      <c r="P9" s="14">
         <f t="shared" si="11"/>
         <v>-0.13033271777671285</v>
       </c>
-      <c r="Q9" s="18">
+      <c r="Q9" s="16">
         <f t="shared" si="12"/>
         <v>-1.7488107104089101E-2</v>
       </c>
-      <c r="R9" s="16">
+      <c r="R9" s="14">
         <f t="shared" si="13"/>
         <v>8.429569847620062</v>
       </c>
-      <c r="S9" s="16">
+      <c r="S9" s="14">
         <f t="shared" si="14"/>
         <v>-0.9769211989714135</v>
       </c>
-      <c r="T9" s="19">
+      <c r="T9" s="17">
         <f t="shared" si="15"/>
         <v>-0.13108375894636515</v>
       </c>
@@ -1763,79 +1749,79 @@
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A10" s="15">
+      <c r="A10" s="13">
         <v>1</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="14">
         <v>7.7386565088757395</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="14">
         <v>0.30965242196380238</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="16">
         <f t="shared" ref="E10:E11" si="16">D10/C10</f>
         <v>4.001371835132507E-2</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="15">
         <f t="shared" ref="F10:F11" si="17">$C$1+X10</f>
         <v>7.6496578665211317</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="14">
         <f t="shared" ref="G10" si="18">$C10-F10</f>
         <v>8.899864235460786E-2</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="16">
         <f t="shared" ref="H10" si="19">1-F10/$C10</f>
         <v>1.150052883889241E-2</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="15">
         <f t="shared" si="4"/>
         <v>7.680572866521131</v>
       </c>
-      <c r="J10" s="16">
+      <c r="J10" s="14">
         <f t="shared" si="5"/>
         <v>5.80836423546085E-2</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="16">
         <f t="shared" si="6"/>
         <v>7.5056493705322191E-3</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10" s="15">
         <f t="shared" ref="L10:L11" si="20">$C$1+Z10</f>
         <v>7.165627450051371</v>
       </c>
-      <c r="M10" s="16">
+      <c r="M10" s="14">
         <f t="shared" ref="M10" si="21">$C10-L10</f>
         <v>0.5730290588243685</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="16">
         <f t="shared" ref="N10" si="22">1-L10/$C10</f>
         <v>7.4047615134118061E-2</v>
       </c>
-      <c r="O10" s="17">
+      <c r="O10" s="15">
         <f t="shared" ref="O10:O11" si="23">$C$1+AA10</f>
         <v>7.5107729982431817</v>
       </c>
-      <c r="P10" s="16">
+      <c r="P10" s="14">
         <f t="shared" ref="P10" si="24">$C10-O10</f>
         <v>0.22788351063255785</v>
       </c>
-      <c r="Q10" s="18">
+      <c r="Q10" s="16">
         <f t="shared" ref="Q10" si="25">1-O10/$C10</f>
         <v>2.9447425450553344E-2</v>
       </c>
-      <c r="R10" s="16">
+      <c r="R10" s="14">
         <f t="shared" ref="R10:R11" si="26">$C$1+AB10</f>
         <v>8.4781679796618405</v>
       </c>
-      <c r="S10" s="16">
+      <c r="S10" s="14">
         <f t="shared" ref="S10" si="27">$C10-R10</f>
         <v>-0.73951147078610102</v>
       </c>
-      <c r="T10" s="19">
+      <c r="T10" s="17">
         <f t="shared" ref="T10" si="28">1-R10/$C10</f>
         <v>-9.5560704876606062E-2</v>
       </c>
@@ -1856,79 +1842,79 @@
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A11" s="15">
+      <c r="A11" s="13">
         <v>1</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="14">
         <v>7.9583879975505205</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="14">
         <v>0.38963995276305119</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="16">
         <f t="shared" si="16"/>
         <v>4.8959657770264134E-2</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="15">
         <f t="shared" si="17"/>
         <v>7.5713312224489711</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="14">
         <f t="shared" ref="G11" si="29">$C11-F11</f>
         <v>0.38705677510154946</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="16">
         <f t="shared" ref="H11" si="30">1-F11/$C11</f>
         <v>4.8635072230793441E-2</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="15">
         <f t="shared" si="4"/>
         <v>7.591268066553071</v>
       </c>
-      <c r="J11" s="16">
+      <c r="J11" s="14">
         <f t="shared" ref="J11" si="31">$C11-I11</f>
         <v>0.36711993099744955</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="16">
         <f t="shared" ref="K11" si="32">1-I11/$C11</f>
         <v>4.6129936252221393E-2</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L11" s="15">
         <f t="shared" si="20"/>
         <v>7.2128543731283008</v>
       </c>
-      <c r="M11" s="16">
+      <c r="M11" s="14">
         <f t="shared" ref="M11" si="33">$C11-L11</f>
         <v>0.74553362442221971</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N11" s="16">
         <f t="shared" ref="N11" si="34">1-L11/$C11</f>
         <v>9.3678974266105719E-2</v>
       </c>
-      <c r="O11" s="17">
+      <c r="O11" s="15">
         <f t="shared" si="23"/>
         <v>7.5849551670717617</v>
       </c>
-      <c r="P11" s="16">
+      <c r="P11" s="14">
         <f t="shared" ref="P11" si="35">$C11-O11</f>
         <v>0.37343283047875886</v>
       </c>
-      <c r="Q11" s="18">
+      <c r="Q11" s="16">
         <f t="shared" ref="Q11" si="36">1-O11/$C11</f>
         <v>4.6923174717505178E-2</v>
       </c>
-      <c r="R11" s="16">
+      <c r="R11" s="14">
         <f t="shared" si="26"/>
         <v>8.5333583762432017</v>
       </c>
-      <c r="S11" s="16">
+      <c r="S11" s="14">
         <f t="shared" ref="S11" si="37">$C11-R11</f>
         <v>-0.57497037869268119</v>
       </c>
-      <c r="T11" s="19">
+      <c r="T11" s="17">
         <f t="shared" ref="T11" si="38">1-R11/$C11</f>
         <v>-7.2247090600464414E-2</v>
       </c>
@@ -1949,79 +1935,79 @@
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A12" s="20">
+      <c r="A12" s="18">
         <v>2</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="19">
         <v>8.1750590818363271</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="19">
         <v>0.1491626477531128</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="21">
         <f t="shared" si="0"/>
         <v>1.8246063577023967E-2</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="20">
         <f t="shared" si="1"/>
         <v>8.0464580654359956</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="19">
         <f t="shared" si="2"/>
         <v>0.1286010164003315</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="21">
         <f t="shared" si="3"/>
         <v>1.5730897491133988E-2</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="20">
         <f t="shared" si="4"/>
         <v>8.0653245429092113</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="19">
         <f t="shared" si="5"/>
         <v>0.10973453892711582</v>
       </c>
-      <c r="K12" s="23">
+      <c r="K12" s="21">
         <f t="shared" si="6"/>
         <v>1.3423088179378206E-2</v>
       </c>
-      <c r="L12" s="22">
+      <c r="L12" s="20">
         <f t="shared" si="7"/>
         <v>7.222382373128303</v>
       </c>
-      <c r="M12" s="21">
+      <c r="M12" s="19">
         <f t="shared" si="8"/>
         <v>0.95267670870802412</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N12" s="21">
         <f t="shared" si="9"/>
         <v>0.11653453500106425</v>
       </c>
-      <c r="O12" s="22">
+      <c r="O12" s="20">
         <f t="shared" si="10"/>
         <v>7.6412987636335314</v>
       </c>
-      <c r="P12" s="21">
+      <c r="P12" s="19">
         <f t="shared" si="11"/>
         <v>0.53376031820279568</v>
       </c>
-      <c r="Q12" s="23">
+      <c r="Q12" s="21">
         <f t="shared" si="12"/>
         <v>6.5291310173980932E-2</v>
       </c>
-      <c r="R12" s="21">
+      <c r="R12" s="19">
         <f t="shared" si="13"/>
         <v>8.762063786435192</v>
       </c>
-      <c r="S12" s="21">
+      <c r="S12" s="19">
         <f t="shared" si="14"/>
         <v>-0.58700470459886489</v>
       </c>
-      <c r="T12" s="24">
+      <c r="T12" s="22">
         <f t="shared" si="15"/>
         <v>-7.1804337891954173E-2</v>
       </c>
@@ -2042,79 +2028,79 @@
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A13" s="20">
+      <c r="A13" s="18">
         <v>2</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="19">
         <v>8.9225564444444441</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="19">
         <v>0.15696522303890859</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="21">
         <f t="shared" si="0"/>
         <v>1.7591956298202146E-2</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="20">
         <f t="shared" si="1"/>
         <v>8.4379379115898416</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="19">
         <f t="shared" si="2"/>
         <v>0.48461853285460244</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="21">
         <f t="shared" si="3"/>
         <v>5.4313865748234713E-2</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="20">
         <f t="shared" si="4"/>
         <v>8.5376591174837202</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="19">
         <f t="shared" si="5"/>
         <v>0.38489732696072387</v>
       </c>
-      <c r="K13" s="23">
+      <c r="K13" s="21">
         <f t="shared" si="6"/>
         <v>4.3137561455313334E-2</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="20">
         <f t="shared" si="7"/>
         <v>7.8964122962052272</v>
       </c>
-      <c r="M13" s="21">
+      <c r="M13" s="19">
         <f t="shared" si="8"/>
         <v>1.0261441482392168</v>
       </c>
-      <c r="N13" s="23">
+      <c r="N13" s="21">
         <f t="shared" si="9"/>
         <v>0.11500562138535275</v>
       </c>
-      <c r="O13" s="22">
+      <c r="O13" s="20">
         <f t="shared" si="10"/>
         <v>8.2167122126762209</v>
       </c>
-      <c r="P13" s="21">
+      <c r="P13" s="19">
         <f t="shared" si="11"/>
         <v>0.7058442317682232</v>
       </c>
-      <c r="Q13" s="23">
+      <c r="Q13" s="21">
         <f t="shared" si="12"/>
         <v>7.9107847191901115E-2</v>
       </c>
-      <c r="R13" s="21">
+      <c r="R13" s="19">
         <f t="shared" si="13"/>
         <v>8.6163971855051908</v>
       </c>
-      <c r="S13" s="21">
+      <c r="S13" s="19">
         <f t="shared" si="14"/>
         <v>0.30615925893925322</v>
       </c>
-      <c r="T13" s="24">
+      <c r="T13" s="22">
         <f t="shared" si="15"/>
         <v>3.4312952890298676E-2</v>
       </c>
@@ -2135,79 +2121,79 @@
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A14" s="20">
+      <c r="A14" s="18">
         <v>2</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="19">
         <v>7.8098835509138373</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="19">
         <v>0.28140906830485357</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="21">
         <f t="shared" si="0"/>
         <v>3.6032428200792548E-2</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="20">
         <f t="shared" si="1"/>
         <v>7.5472798346667656</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="19">
         <f t="shared" si="2"/>
         <v>0.26260371624707179</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="21">
         <f t="shared" si="3"/>
         <v>3.3624536721337472E-2</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="20">
         <f t="shared" si="4"/>
         <v>7.5820333737105212</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="19">
         <f t="shared" si="5"/>
         <v>0.22785017720331613</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="21">
         <f t="shared" si="6"/>
         <v>2.9174593413323735E-2</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="20">
         <f t="shared" si="7"/>
         <v>7.166231065435996</v>
       </c>
-      <c r="M14" s="21">
+      <c r="M14" s="19">
         <f t="shared" si="8"/>
         <v>0.64365248547784137</v>
       </c>
-      <c r="N14" s="23">
+      <c r="N14" s="21">
         <f t="shared" si="9"/>
         <v>8.2415119416540783E-2</v>
       </c>
-      <c r="O14" s="22">
+      <c r="O14" s="20">
         <f t="shared" si="10"/>
         <v>7.5991695113384514</v>
       </c>
-      <c r="P14" s="21">
+      <c r="P14" s="19">
         <f t="shared" si="11"/>
         <v>0.21071403957538593</v>
       </c>
-      <c r="Q14" s="23">
+      <c r="Q14" s="21">
         <f t="shared" si="12"/>
         <v>2.698043296058239E-2</v>
       </c>
-      <c r="R14" s="21">
+      <c r="R14" s="19">
         <f t="shared" si="13"/>
         <v>8.6191512358207607</v>
       </c>
-      <c r="S14" s="21">
+      <c r="S14" s="19">
         <f t="shared" si="14"/>
         <v>-0.80926768490692336</v>
       </c>
-      <c r="T14" s="24">
+      <c r="T14" s="22">
         <f t="shared" si="15"/>
         <v>-0.103620966898057</v>
       </c>
@@ -2228,79 +2214,79 @@
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A15" s="20">
+      <c r="A15" s="18">
         <v>2</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="19">
         <v>8.0508098305084737</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="19">
         <v>0.4134573880918902</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="21">
         <f t="shared" ref="E15:E16" si="39">D15/C15</f>
         <v>5.135599980577072E-2</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="20">
         <f t="shared" ref="F15:F16" si="40">$C$1+X15</f>
         <v>7.808873542709601</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="19">
         <f t="shared" ref="G15" si="41">$C15-F15</f>
         <v>0.24193628779887266</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="21">
         <f t="shared" ref="H15" si="42">1-F15/$C15</f>
         <v>3.0051174092084132E-2</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="20">
         <f t="shared" si="4"/>
         <v>7.8469500677698107</v>
       </c>
-      <c r="J15" s="21">
+      <c r="J15" s="19">
         <f t="shared" si="5"/>
         <v>0.20385976273866291</v>
       </c>
-      <c r="K15" s="23">
+      <c r="K15" s="21">
         <f t="shared" si="6"/>
         <v>2.5321646769762007E-2</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="20">
         <f t="shared" ref="L15:L16" si="43">$C$1+Z15</f>
         <v>7.1316789115898409</v>
       </c>
-      <c r="M15" s="21">
+      <c r="M15" s="19">
         <f t="shared" ref="M15" si="44">$C15-L15</f>
         <v>0.91913091891863274</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N15" s="21">
         <f t="shared" ref="N15" si="45">1-L15/$C15</f>
         <v>0.11416626876908631</v>
       </c>
-      <c r="O15" s="22">
+      <c r="O15" s="20">
         <f t="shared" ref="O15:O16" si="46">$C$1+AA15</f>
         <v>7.5485898544257211</v>
       </c>
-      <c r="P15" s="21">
+      <c r="P15" s="19">
         <f t="shared" ref="P15" si="47">$C15-O15</f>
         <v>0.50221997608275259</v>
       </c>
-      <c r="Q15" s="23">
+      <c r="Q15" s="21">
         <f t="shared" ref="Q15" si="48">1-O15/$C15</f>
         <v>6.2381299106034627E-2</v>
       </c>
-      <c r="R15" s="21">
+      <c r="R15" s="19">
         <f t="shared" ref="R15:R16" si="49">$C$1+AB15</f>
         <v>8.6991157235568117</v>
       </c>
-      <c r="S15" s="21">
+      <c r="S15" s="19">
         <f t="shared" ref="S15" si="50">$C15-R15</f>
         <v>-0.64830589304833808</v>
       </c>
-      <c r="T15" s="24">
+      <c r="T15" s="22">
         <f t="shared" ref="T15" si="51">1-R15/$C15</f>
         <v>-8.0526792545960957E-2</v>
       </c>
@@ -2321,79 +2307,79 @@
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A16" s="20">
+      <c r="A16" s="18">
         <v>2</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="19">
         <v>7.6933738053097347</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="19">
         <v>0.25430941639396804</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="21">
         <f t="shared" si="39"/>
         <v>3.3055642794641196E-2</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="20">
         <f t="shared" si="40"/>
         <v>7.5799491754084709</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="19">
         <f t="shared" ref="G16" si="52">$C16-F16</f>
         <v>0.11342462990126378</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="21">
         <f t="shared" ref="H16" si="53">1-F16/$C16</f>
         <v>1.4743158563669589E-2</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="20">
         <f t="shared" si="4"/>
         <v>7.6233968004386909</v>
       </c>
-      <c r="J16" s="21">
+      <c r="J16" s="19">
         <f t="shared" ref="J16" si="54">$C16-I16</f>
         <v>6.9977004871043746E-2</v>
       </c>
-      <c r="K16" s="23">
+      <c r="K16" s="21">
         <f t="shared" ref="K16" si="55">1-I16/$C16</f>
         <v>9.0957500105802724E-3</v>
       </c>
-      <c r="L16" s="22">
+      <c r="L16" s="20">
         <f t="shared" si="43"/>
         <v>7.1749688346667613</v>
       </c>
-      <c r="M16" s="21">
+      <c r="M16" s="19">
         <f t="shared" ref="M16" si="56">$C16-L16</f>
         <v>0.51840497064297342</v>
       </c>
-      <c r="N16" s="23">
+      <c r="N16" s="21">
         <f t="shared" ref="N16" si="57">1-L16/$C16</f>
         <v>6.738330721499397E-2</v>
       </c>
-      <c r="O16" s="22">
+      <c r="O16" s="20">
         <f t="shared" si="46"/>
         <v>7.6215743117043413</v>
       </c>
-      <c r="P16" s="21">
+      <c r="P16" s="19">
         <f t="shared" ref="P16" si="58">$C16-O16</f>
         <v>7.1799493605393394E-2</v>
       </c>
-      <c r="Q16" s="23">
+      <c r="Q16" s="21">
         <f t="shared" ref="Q16" si="59">1-O16/$C16</f>
         <v>9.332640714251994E-3</v>
       </c>
-      <c r="R16" s="21">
+      <c r="R16" s="19">
         <f t="shared" si="49"/>
         <v>8.6567929409099307</v>
       </c>
-      <c r="S16" s="21">
+      <c r="S16" s="19">
         <f t="shared" ref="S16" si="60">$C16-R16</f>
         <v>-0.96341913560019599</v>
       </c>
-      <c r="T16" s="24">
+      <c r="T16" s="22">
         <f t="shared" ref="T16" si="61">1-R16/$C16</f>
         <v>-0.12522713181247913</v>
       </c>
@@ -2414,79 +2400,79 @@
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A17" s="25">
+      <c r="A17" s="23">
         <v>3</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="24">
         <v>8.1864021653543304</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="24">
         <v>0.30290167558805503</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="26">
         <f t="shared" si="0"/>
         <v>3.7000585784798735E-2</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="25">
         <f t="shared" si="1"/>
         <v>8.1256968346667655</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="24">
         <f t="shared" si="2"/>
         <v>6.0705330687564896E-2</v>
       </c>
-      <c r="H17" s="28">
+      <c r="H17" s="26">
         <f t="shared" si="3"/>
         <v>7.4153858387846494E-3</v>
       </c>
-      <c r="I17" s="27">
+      <c r="I17" s="25">
         <f t="shared" si="4"/>
         <v>8.1368539370180208</v>
       </c>
-      <c r="J17" s="26">
+      <c r="J17" s="24">
         <f t="shared" si="5"/>
         <v>4.9548228336309563E-2</v>
       </c>
-      <c r="K17" s="28">
+      <c r="K17" s="26">
         <f t="shared" si="6"/>
         <v>6.0525035706164854E-3</v>
       </c>
-      <c r="L17" s="27">
+      <c r="L17" s="25">
         <f t="shared" si="7"/>
         <v>7.4797047577436881</v>
       </c>
-      <c r="M17" s="26">
+      <c r="M17" s="24">
         <f t="shared" si="8"/>
         <v>0.70669740761064226</v>
       </c>
-      <c r="N17" s="28">
+      <c r="N17" s="26">
         <f t="shared" si="9"/>
         <v>8.6325762323460786E-2</v>
       </c>
-      <c r="O17" s="27">
+      <c r="O17" s="25">
         <f t="shared" si="10"/>
         <v>7.9129264232162813</v>
       </c>
-      <c r="P17" s="26">
+      <c r="P17" s="24">
         <f t="shared" si="11"/>
         <v>0.27347574213804915</v>
       </c>
-      <c r="Q17" s="28">
+      <c r="Q17" s="26">
         <f t="shared" si="12"/>
         <v>3.3406096672775942E-2</v>
       </c>
-      <c r="R17" s="26">
+      <c r="R17" s="24">
         <f t="shared" si="13"/>
         <v>9.0543814225513906</v>
       </c>
-      <c r="S17" s="26">
+      <c r="S17" s="24">
         <f t="shared" si="14"/>
         <v>-0.86797925719706015</v>
       </c>
-      <c r="T17" s="29">
+      <c r="T17" s="27">
         <f t="shared" si="15"/>
         <v>-0.10602695050463495</v>
       </c>
@@ -2507,79 +2493,79 @@
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A18" s="25">
+      <c r="A18" s="23">
         <v>3</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="24">
         <v>8.9912262443438919</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="24">
         <v>0.24958836271839085</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18" s="26">
         <f t="shared" si="0"/>
         <v>2.7759101588106443E-2</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="25">
         <f t="shared" si="1"/>
         <v>8.6220155269744581</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="24">
         <f t="shared" si="2"/>
         <v>0.36921071736943389</v>
       </c>
-      <c r="H18" s="28">
+      <c r="H18" s="26">
         <f t="shared" si="3"/>
         <v>4.1063444221714818E-2</v>
       </c>
-      <c r="I18" s="27">
+      <c r="I18" s="25">
         <f t="shared" si="4"/>
         <v>8.7004929850560107</v>
       </c>
-      <c r="J18" s="26">
+      <c r="J18" s="24">
         <f t="shared" si="5"/>
         <v>0.2907332592878813</v>
       </c>
-      <c r="K18" s="28">
+      <c r="K18" s="26">
         <f t="shared" si="6"/>
         <v>3.2335217843147079E-2</v>
       </c>
-      <c r="L18" s="27">
+      <c r="L18" s="25">
         <f t="shared" si="7"/>
         <v>8.1140244500513816</v>
       </c>
-      <c r="M18" s="26">
+      <c r="M18" s="24">
         <f t="shared" si="8"/>
         <v>0.87720179429251033</v>
       </c>
-      <c r="N18" s="28">
+      <c r="N18" s="26">
         <f t="shared" si="9"/>
         <v>9.7561975469623086E-2</v>
       </c>
-      <c r="O18" s="27">
+      <c r="O18" s="25">
         <f t="shared" si="10"/>
         <v>8.4903397637975715</v>
       </c>
-      <c r="P18" s="26">
+      <c r="P18" s="24">
         <f t="shared" si="11"/>
         <v>0.50088648054632046</v>
       </c>
-      <c r="Q18" s="28">
+      <c r="Q18" s="26">
         <f t="shared" si="12"/>
         <v>5.5708361344083968E-2</v>
       </c>
-      <c r="R18" s="26">
+      <c r="R18" s="24">
         <f t="shared" si="13"/>
         <v>9.0195559095452715</v>
       </c>
-      <c r="S18" s="26">
+      <c r="S18" s="24">
         <f t="shared" si="14"/>
         <v>-2.8329665201379584E-2</v>
       </c>
-      <c r="T18" s="29">
+      <c r="T18" s="27">
         <f t="shared" si="15"/>
         <v>-3.150812184177898E-3</v>
       </c>
@@ -2600,79 +2586,79 @@
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A19" s="25">
+      <c r="A19" s="23">
         <v>3</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="24">
         <v>8.1900440239043828</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="24">
         <v>0.20398054945489216</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="26">
         <f t="shared" si="0"/>
         <v>2.4905916117121178E-2</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="25">
         <f t="shared" si="1"/>
         <v>7.7252361423590727</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="24">
         <f t="shared" si="2"/>
         <v>0.46480788154531005</v>
       </c>
-      <c r="H19" s="28">
+      <c r="H19" s="26">
         <f t="shared" si="3"/>
         <v>5.6752794025119901E-2</v>
       </c>
-      <c r="I19" s="27">
+      <c r="I19" s="25">
         <f t="shared" si="4"/>
         <v>7.759048114932221</v>
       </c>
-      <c r="J19" s="26">
+      <c r="J19" s="24">
         <f t="shared" si="5"/>
         <v>0.43099590897216178</v>
       </c>
-      <c r="K19" s="28">
+      <c r="K19" s="26">
         <f t="shared" si="6"/>
         <v>5.262437023710842E-2</v>
       </c>
-      <c r="L19" s="27">
+      <c r="L19" s="25">
         <f t="shared" si="7"/>
         <v>7.25007545005138</v>
       </c>
-      <c r="M19" s="26">
+      <c r="M19" s="24">
         <f t="shared" si="8"/>
         <v>0.93996857385300281</v>
       </c>
-      <c r="N19" s="28">
+      <c r="N19" s="26">
         <f t="shared" si="9"/>
         <v>0.11476966071360606</v>
       </c>
-      <c r="O19" s="27">
+      <c r="O19" s="25">
         <f t="shared" si="10"/>
         <v>7.6968433632552316</v>
       </c>
-      <c r="P19" s="26">
+      <c r="P19" s="24">
         <f t="shared" si="11"/>
         <v>0.49320066064915125</v>
       </c>
-      <c r="Q19" s="28">
+      <c r="Q19" s="26">
         <f t="shared" si="12"/>
         <v>6.0219537185592698E-2</v>
       </c>
-      <c r="R19" s="26">
+      <c r="R19" s="24">
         <f t="shared" si="13"/>
         <v>8.9698741513115721</v>
       </c>
-      <c r="S19" s="26">
+      <c r="S19" s="24">
         <f t="shared" si="14"/>
         <v>-0.77983012740718927</v>
       </c>
-      <c r="T19" s="29">
+      <c r="T19" s="27">
         <f t="shared" si="15"/>
         <v>-9.5216841952386222E-2</v>
       </c>
@@ -2693,79 +2679,79 @@
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A20" s="25">
+      <c r="A20" s="23">
         <v>3</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="24">
         <v>8.2021879799666113</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="24">
         <v>0.33652739631399425</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E20" s="26">
         <f t="shared" si="0"/>
         <v>4.1028978747615116E-2</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="25">
         <f t="shared" ref="F20:F21" si="62">$C$1+X20</f>
         <v>7.9040848469982414</v>
       </c>
-      <c r="G20" s="26">
+      <c r="G20" s="24">
         <f t="shared" ref="G20" si="63">$C20-F20</f>
         <v>0.29810313296836988</v>
       </c>
-      <c r="H20" s="28">
+      <c r="H20" s="26">
         <f t="shared" ref="H20" si="64">1-F20/$C20</f>
         <v>3.6344342960252796E-2</v>
       </c>
-      <c r="I20" s="27">
+      <c r="I20" s="25">
         <f t="shared" si="4"/>
         <v>7.9040848469982414</v>
       </c>
-      <c r="J20" s="26">
+      <c r="J20" s="24">
         <f t="shared" si="5"/>
         <v>0.29810313296836988</v>
       </c>
-      <c r="K20" s="28">
+      <c r="K20" s="26">
         <f t="shared" si="6"/>
         <v>3.6344342960252796E-2</v>
       </c>
-      <c r="L20" s="27">
+      <c r="L20" s="25">
         <f t="shared" ref="L20:L21" si="65">$C$1+Z20</f>
         <v>7.2377742192821408</v>
       </c>
-      <c r="M20" s="26">
+      <c r="M20" s="24">
         <f t="shared" ref="M20" si="66">$C20-L20</f>
         <v>0.96441376068447049</v>
       </c>
-      <c r="N20" s="28">
+      <c r="N20" s="26">
         <f t="shared" ref="N20" si="67">1-L20/$C20</f>
         <v>0.11758006071550631</v>
       </c>
-      <c r="O20" s="27">
+      <c r="O20" s="25">
         <f t="shared" ref="O20:O21" si="68">$C$1+AA20</f>
         <v>7.6857938481775312</v>
       </c>
-      <c r="P20" s="26">
+      <c r="P20" s="24">
         <f t="shared" ref="P20" si="69">$C20-O20</f>
         <v>0.51639413178908011</v>
       </c>
-      <c r="Q20" s="28">
+      <c r="Q20" s="26">
         <f t="shared" ref="Q20" si="70">1-O20/$C20</f>
         <v>6.2958095211953724E-2</v>
       </c>
-      <c r="R20" s="26">
+      <c r="R20" s="24">
         <f t="shared" ref="R20:R21" si="71">$C$1+AB20</f>
         <v>8.9974887895323707</v>
       </c>
-      <c r="S20" s="26">
+      <c r="S20" s="24">
         <f t="shared" ref="S20" si="72">$C20-R20</f>
         <v>-0.79530080956575944</v>
       </c>
-      <c r="T20" s="29">
+      <c r="T20" s="27">
         <f t="shared" ref="T20" si="73">1-R20/$C20</f>
         <v>-9.6962031534541415E-2</v>
       </c>
@@ -2786,79 +2772,79 @@
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A21" s="25">
+      <c r="A21" s="23">
         <v>3</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="24">
         <v>8.0739918406072118</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="24">
         <v>0.26954324280840547</v>
       </c>
-      <c r="E21" s="28">
+      <c r="E21" s="26">
         <f t="shared" si="0"/>
         <v>3.3384136141031105E-2</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F21" s="25">
         <f t="shared" si="62"/>
         <v>7.7404729826697709</v>
       </c>
-      <c r="G21" s="26">
+      <c r="G21" s="24">
         <f t="shared" ref="G21" si="74">$C21-F21</f>
         <v>0.33351885793744085</v>
       </c>
-      <c r="H21" s="28">
+      <c r="H21" s="26">
         <f t="shared" ref="H21" si="75">1-F21/$C21</f>
         <v>4.1307802202628752E-2</v>
       </c>
-      <c r="I21" s="27">
+      <c r="I21" s="25">
         <f t="shared" si="4"/>
         <v>7.7571195211313118</v>
       </c>
-      <c r="J21" s="26">
+      <c r="J21" s="24">
         <f t="shared" ref="J21" si="76">$C21-I21</f>
         <v>0.3168723194759</v>
       </c>
-      <c r="K21" s="28">
+      <c r="K21" s="26">
         <f t="shared" ref="K21" si="77">1-I21/$C21</f>
         <v>3.9246053963322924E-2</v>
       </c>
-      <c r="L21" s="27">
+      <c r="L21" s="25">
         <f t="shared" si="65"/>
         <v>7.2500754500513711</v>
       </c>
-      <c r="M21" s="26">
+      <c r="M21" s="24">
         <f t="shared" ref="M21" si="78">$C21-L21</f>
         <v>0.82391639055584065</v>
       </c>
-      <c r="N21" s="28">
+      <c r="N21" s="26">
         <f t="shared" ref="N21" si="79">1-L21/$C21</f>
         <v>0.10204572989683347</v>
       </c>
-      <c r="O21" s="27">
+      <c r="O21" s="25">
         <f t="shared" si="68"/>
         <v>7.7127764786398405</v>
       </c>
-      <c r="P21" s="26">
+      <c r="P21" s="24">
         <f t="shared" ref="P21" si="80">$C21-O21</f>
         <v>0.36121536196737125</v>
       </c>
-      <c r="Q21" s="28">
+      <c r="Q21" s="26">
         <f t="shared" ref="Q21" si="81">1-O21/$C21</f>
         <v>4.4738138098019853E-2</v>
       </c>
-      <c r="R21" s="26">
+      <c r="R21" s="24">
         <f t="shared" si="71"/>
         <v>9.0017403820808006</v>
       </c>
-      <c r="S21" s="26">
+      <c r="S21" s="24">
         <f t="shared" ref="S21" si="82">$C21-R21</f>
         <v>-0.92774854147358887</v>
       </c>
-      <c r="T21" s="29">
+      <c r="T21" s="27">
         <f t="shared" ref="T21" si="83">1-R21/$C21</f>
         <v>-0.11490580617230561</v>
       </c>
@@ -2879,79 +2865,79 @@
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A22" s="30">
+      <c r="A22" s="28">
         <v>4</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C22" s="29">
         <v>7.4630859289617479</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="29">
         <v>0.2783420640340748</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="31">
         <f t="shared" si="0"/>
         <v>3.7295840713011501E-2</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F22" s="30">
         <f t="shared" si="1"/>
         <v>8.0267967641539446</v>
       </c>
-      <c r="G22" s="31">
+      <c r="G22" s="29">
         <f t="shared" si="2"/>
         <v>-0.56371083519219667</v>
       </c>
-      <c r="H22" s="33">
+      <c r="H22" s="31">
         <f t="shared" si="3"/>
         <v>-7.5533209795243472E-2</v>
       </c>
-      <c r="I22" s="32">
+      <c r="I22" s="30">
         <f t="shared" si="4"/>
         <v>8.1264635873434212</v>
       </c>
-      <c r="J22" s="31">
+      <c r="J22" s="29">
         <f t="shared" si="5"/>
         <v>-0.66337765838167329</v>
       </c>
-      <c r="K22" s="33">
+      <c r="K22" s="31">
         <f t="shared" si="6"/>
         <v>-8.8887849436025679E-2</v>
       </c>
-      <c r="L22" s="32">
+      <c r="L22" s="30">
         <f t="shared" si="7"/>
         <v>7.134401680820611</v>
       </c>
-      <c r="M22" s="31">
+      <c r="M22" s="29">
         <f t="shared" si="8"/>
         <v>0.32868424814113695</v>
       </c>
-      <c r="N22" s="33">
+      <c r="N22" s="31">
         <f t="shared" si="9"/>
         <v>4.4041332401871802E-2</v>
       </c>
-      <c r="O22" s="32">
+      <c r="O22" s="30">
         <f t="shared" si="10"/>
         <v>7.5492793722859011</v>
       </c>
-      <c r="P22" s="31">
+      <c r="P22" s="29">
         <f t="shared" si="11"/>
         <v>-8.6193443324153129E-2</v>
       </c>
-      <c r="Q22" s="33">
+      <c r="Q22" s="31">
         <f t="shared" si="12"/>
         <v>-1.1549303350463225E-2</v>
       </c>
-      <c r="R22" s="31">
+      <c r="R22" s="29">
         <f t="shared" si="13"/>
         <v>8.3833663804523404</v>
       </c>
-      <c r="S22" s="31">
+      <c r="S22" s="29">
         <f t="shared" si="14"/>
         <v>-0.92028045149059245</v>
       </c>
-      <c r="T22" s="34">
+      <c r="T22" s="32">
         <f t="shared" si="15"/>
         <v>-0.12331098157657427</v>
       </c>
@@ -2972,79 +2958,79 @@
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A23" s="30">
+      <c r="A23" s="28">
         <v>4</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="31">
+      <c r="C23" s="29">
         <v>8.1467038674033159</v>
       </c>
-      <c r="D23" s="31">
+      <c r="D23" s="29">
         <v>0.20731566300858609</v>
       </c>
-      <c r="E23" s="33">
+      <c r="E23" s="31">
         <f t="shared" si="0"/>
         <v>2.5447796603740549E-2</v>
       </c>
-      <c r="F23" s="32">
+      <c r="F23" s="30">
         <f t="shared" si="1"/>
         <v>8.2816591808206113</v>
       </c>
-      <c r="G23" s="31">
+      <c r="G23" s="29">
         <f t="shared" si="2"/>
         <v>-0.13495531341729539</v>
       </c>
-      <c r="H23" s="33">
+      <c r="H23" s="31">
         <f t="shared" si="3"/>
         <v>-1.6565633858041773E-2</v>
       </c>
-      <c r="I23" s="32">
+      <c r="I23" s="30">
         <f t="shared" si="4"/>
         <v>8.3687372180550117</v>
       </c>
-      <c r="J23" s="31">
+      <c r="J23" s="29">
         <f t="shared" si="5"/>
         <v>-0.22203335065169583</v>
       </c>
-      <c r="K23" s="33">
+      <c r="K23" s="31">
         <f t="shared" si="6"/>
         <v>-2.7254378490434439E-2</v>
       </c>
-      <c r="L23" s="32">
+      <c r="L23" s="30">
         <f t="shared" si="7"/>
         <v>7.9350504308206116</v>
       </c>
-      <c r="M23" s="31">
+      <c r="M23" s="29">
         <f t="shared" si="8"/>
         <v>0.2116534365827043</v>
       </c>
-      <c r="N23" s="33">
+      <c r="N23" s="31">
         <f t="shared" si="9"/>
         <v>2.5980254103696421E-2</v>
       </c>
-      <c r="O23" s="32">
+      <c r="O23" s="30">
         <f t="shared" si="10"/>
         <v>8.1284530422837307</v>
       </c>
-      <c r="P23" s="31">
+      <c r="P23" s="29">
         <f t="shared" si="11"/>
         <v>1.8250825119585201E-2</v>
       </c>
-      <c r="Q23" s="33">
+      <c r="Q23" s="31">
         <f t="shared" si="12"/>
         <v>2.240271085906409E-3</v>
       </c>
-      <c r="R23" s="31">
+      <c r="R23" s="29">
         <f t="shared" si="13"/>
         <v>8.3607343843141617</v>
       </c>
-      <c r="S23" s="31">
+      <c r="S23" s="29">
         <f t="shared" si="14"/>
         <v>-0.21403051691084585</v>
       </c>
-      <c r="T23" s="34">
+      <c r="T23" s="32">
         <f t="shared" si="15"/>
         <v>-2.6272038408960308E-2</v>
       </c>
@@ -3065,79 +3051,79 @@
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A24" s="30">
+      <c r="A24" s="28">
         <v>4</v>
       </c>
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="31">
+      <c r="C24" s="29">
         <v>7.2364042292710069</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="29">
         <v>0.27489160416221231</v>
       </c>
-      <c r="E24" s="33">
+      <c r="E24" s="31">
         <f t="shared" si="0"/>
         <v>3.7987320145865429E-2</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="30">
         <f t="shared" si="1"/>
         <v>7.4424792641539446</v>
       </c>
-      <c r="G24" s="31">
+      <c r="G24" s="29">
         <f t="shared" si="2"/>
         <v>-0.20607503488293766</v>
       </c>
-      <c r="H24" s="33">
+      <c r="H24" s="31">
         <f t="shared" si="3"/>
         <v>-2.8477546078668592E-2</v>
       </c>
-      <c r="I24" s="32">
+      <c r="I24" s="30">
         <f t="shared" si="4"/>
         <v>7.4785280135136114</v>
       </c>
-      <c r="J24" s="31">
+      <c r="J24" s="29">
         <f t="shared" si="5"/>
         <v>-0.2421237842426045</v>
       </c>
-      <c r="K24" s="33">
+      <c r="K24" s="31">
         <f t="shared" si="6"/>
         <v>-3.3459129226532491E-2</v>
       </c>
-      <c r="L24" s="32">
+      <c r="L24" s="30">
         <f t="shared" si="7"/>
         <v>7.0731279308206112</v>
       </c>
-      <c r="M24" s="31">
+      <c r="M24" s="29">
         <f t="shared" si="8"/>
         <v>0.16327629845039571</v>
       </c>
-      <c r="N24" s="33">
+      <c r="N24" s="31">
         <f t="shared" si="9"/>
         <v>2.2563181005000876E-2</v>
       </c>
-      <c r="O24" s="32">
+      <c r="O24" s="30">
         <f t="shared" si="10"/>
         <v>7.4170550388195613</v>
       </c>
-      <c r="P24" s="31">
+      <c r="P24" s="29">
         <f t="shared" si="11"/>
         <v>-0.18065080954855439</v>
       </c>
-      <c r="Q24" s="33">
+      <c r="Q24" s="31">
         <f t="shared" si="12"/>
         <v>-2.4964167813874782E-2</v>
       </c>
-      <c r="R24" s="31">
+      <c r="R24" s="29">
         <f t="shared" si="13"/>
         <v>8.2295084702911208</v>
       </c>
-      <c r="S24" s="31">
+      <c r="S24" s="29">
         <f t="shared" si="14"/>
         <v>-0.99310424102011385</v>
       </c>
-      <c r="T24" s="34">
+      <c r="T24" s="32">
         <f t="shared" si="15"/>
         <v>-0.13723725341420834</v>
       </c>
@@ -3158,79 +3144,79 @@
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A25" s="30">
+      <c r="A25" s="28">
         <v>4</v>
       </c>
-      <c r="B25" s="52" t="s">
+      <c r="B25" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="31">
+      <c r="C25" s="29">
         <v>7.7085365122615803</v>
       </c>
-      <c r="D25" s="31">
+      <c r="D25" s="29">
         <v>0.3752050982843535</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="31">
         <f t="shared" si="0"/>
         <v>4.8673973028153093E-2</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="30">
         <f t="shared" ref="F25:F26" si="84">$C$1+X25</f>
         <v>7.5408011918333413</v>
       </c>
-      <c r="G25" s="31">
+      <c r="G25" s="29">
         <f t="shared" ref="G25" si="85">$C25-F25</f>
         <v>0.16773532042823902</v>
       </c>
-      <c r="H25" s="33">
+      <c r="H25" s="31">
         <f t="shared" ref="H25" si="86">1-F25/$C25</f>
         <v>2.1759684235967636E-2</v>
       </c>
-      <c r="I25" s="32">
+      <c r="I25" s="30">
         <f t="shared" si="4"/>
         <v>7.557183035911641</v>
       </c>
-      <c r="J25" s="31">
+      <c r="J25" s="29">
         <f t="shared" si="5"/>
         <v>0.15135347634993934</v>
       </c>
-      <c r="K25" s="33">
+      <c r="K25" s="31">
         <f t="shared" si="6"/>
         <v>1.9634528046820421E-2</v>
       </c>
-      <c r="L25" s="32">
+      <c r="L25" s="30">
         <f t="shared" ref="L25:L26" si="87">$C$1+Z25</f>
         <v>7.0654755974872714</v>
       </c>
-      <c r="M25" s="31">
+      <c r="M25" s="29">
         <f t="shared" ref="M25" si="88">$C25-L25</f>
         <v>0.64306091477430893</v>
       </c>
-      <c r="N25" s="33">
+      <c r="N25" s="31">
         <f t="shared" ref="N25" si="89">1-L25/$C25</f>
         <v>8.3421919809476774E-2</v>
       </c>
-      <c r="O25" s="32">
+      <c r="O25" s="30">
         <f t="shared" ref="O25:O26" si="90">$C$1+AA25</f>
         <v>7.3705687900295809</v>
       </c>
-      <c r="P25" s="31">
+      <c r="P25" s="29">
         <f t="shared" ref="P25" si="91">$C25-O25</f>
         <v>0.33796772223199945</v>
       </c>
-      <c r="Q25" s="33">
+      <c r="Q25" s="31">
         <f t="shared" ref="Q25" si="92">1-O25/$C25</f>
         <v>4.3843305625446694E-2</v>
       </c>
-      <c r="R25" s="31">
+      <c r="R25" s="29">
         <f t="shared" ref="R25:R26" si="93">$C$1+AB25</f>
         <v>8.2240995803169614</v>
       </c>
-      <c r="S25" s="31">
+      <c r="S25" s="29">
         <f t="shared" ref="S25" si="94">$C25-R25</f>
         <v>-0.5155630680553811</v>
       </c>
-      <c r="T25" s="34">
+      <c r="T25" s="32">
         <f t="shared" ref="T25" si="95">1-R25/$C25</f>
         <v>-6.6882094575968054E-2</v>
       </c>
@@ -3251,79 +3237,79 @@
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A26" s="30">
+      <c r="A26" s="28">
         <v>4</v>
       </c>
-      <c r="B26" s="52" t="s">
+      <c r="B26" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="31">
+      <c r="C26" s="29">
         <v>7.5108153918791309</v>
       </c>
-      <c r="D26" s="31">
+      <c r="D26" s="29">
         <v>0.27419899725124913</v>
       </c>
-      <c r="E26" s="33">
+      <c r="E26" s="31">
         <f t="shared" si="0"/>
         <v>3.6507220979990998E-2</v>
       </c>
-      <c r="F26" s="32">
+      <c r="F26" s="30">
         <f t="shared" si="84"/>
         <v>7.4556441581838708</v>
       </c>
-      <c r="G26" s="31">
+      <c r="G26" s="29">
         <f t="shared" ref="G26" si="96">$C26-F26</f>
         <v>5.5171233695260113E-2</v>
       </c>
-      <c r="H26" s="33">
+      <c r="H26" s="31">
         <f t="shared" ref="H26" si="97">1-F26/$C26</f>
         <v>7.3455717943636811E-3</v>
       </c>
-      <c r="I26" s="32">
+      <c r="I26" s="30">
         <f t="shared" si="4"/>
         <v>7.5143036514230008</v>
       </c>
-      <c r="J26" s="31">
+      <c r="J26" s="29">
         <f t="shared" ref="J26" si="98">$C26-I26</f>
         <v>-3.4882595438698871E-3</v>
       </c>
-      <c r="K26" s="33">
+      <c r="K26" s="31">
         <f t="shared" ref="K26" si="99">1-I26/$C26</f>
         <v>-4.6443153797137704E-4</v>
       </c>
-      <c r="L26" s="32">
+      <c r="L26" s="30">
         <f t="shared" si="87"/>
         <v>7.113518347487271</v>
       </c>
-      <c r="M26" s="31">
+      <c r="M26" s="29">
         <f t="shared" ref="M26" si="100">$C26-L26</f>
         <v>0.39729704439185998</v>
       </c>
-      <c r="N26" s="33">
+      <c r="N26" s="31">
         <f t="shared" ref="N26" si="101">1-L26/$C26</f>
         <v>5.2896659505361709E-2</v>
       </c>
-      <c r="O26" s="32">
+      <c r="O26" s="30">
         <f t="shared" si="90"/>
         <v>7.4662583771204911</v>
       </c>
-      <c r="P26" s="31">
+      <c r="P26" s="29">
         <f t="shared" ref="P26" si="102">$C26-O26</f>
         <v>4.4557014758639824E-2</v>
       </c>
-      <c r="Q26" s="33">
+      <c r="Q26" s="31">
         <f t="shared" ref="Q26" si="103">1-O26/$C26</f>
         <v>5.932380498502976E-3</v>
       </c>
-      <c r="R26" s="31">
+      <c r="R26" s="29">
         <f t="shared" si="93"/>
         <v>8.2612371399956217</v>
       </c>
-      <c r="S26" s="31">
+      <c r="S26" s="29">
         <f t="shared" ref="S26" si="104">$C26-R26</f>
         <v>-0.75042174811649076</v>
       </c>
-      <c r="T26" s="34">
+      <c r="T26" s="32">
         <f t="shared" ref="T26" si="105">1-R26/$C26</f>
         <v>-9.9912154534894437E-2</v>
       </c>
@@ -3344,79 +3330,79 @@
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A27" s="35">
+      <c r="A27" s="33">
         <v>5</v>
       </c>
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="36">
+      <c r="C27" s="34">
         <v>8.199037379576108</v>
       </c>
-      <c r="D27" s="36">
+      <c r="D27" s="34">
         <v>0.25509964109722122</v>
       </c>
-      <c r="E27" s="38">
+      <c r="E27" s="36">
         <f t="shared" si="0"/>
         <v>3.1113364811907948E-2</v>
       </c>
-      <c r="F27" s="37">
+      <c r="F27" s="35">
         <f t="shared" si="1"/>
         <v>8.2131679885129181</v>
       </c>
-      <c r="G27" s="36">
+      <c r="G27" s="34">
         <f t="shared" si="2"/>
         <v>-1.4130608936810063E-2</v>
       </c>
-      <c r="H27" s="38">
+      <c r="H27" s="36">
         <f t="shared" si="3"/>
         <v>-1.7234473124869698E-3</v>
       </c>
-      <c r="I27" s="37">
+      <c r="I27" s="35">
         <f t="shared" si="4"/>
         <v>8.2661993885649512</v>
       </c>
-      <c r="J27" s="36">
+      <c r="J27" s="34">
         <f t="shared" si="5"/>
         <v>-6.7162008988843169E-2</v>
       </c>
-      <c r="K27" s="38">
+      <c r="K27" s="36">
         <f t="shared" si="6"/>
         <v>-8.1914505178553032E-3</v>
       </c>
-      <c r="L27" s="37">
+      <c r="L27" s="35">
         <f t="shared" si="7"/>
         <v>7.2936038346667651</v>
       </c>
-      <c r="M27" s="36">
+      <c r="M27" s="34">
         <f t="shared" si="8"/>
         <v>0.90543354490934291</v>
       </c>
-      <c r="N27" s="38">
+      <c r="N27" s="36">
         <f t="shared" si="9"/>
         <v>0.11043168886688914</v>
       </c>
-      <c r="O27" s="37">
+      <c r="O27" s="35">
         <f t="shared" si="10"/>
         <v>8.02679642725926</v>
       </c>
-      <c r="P27" s="36">
+      <c r="P27" s="34">
         <f t="shared" si="11"/>
         <v>0.172240952316848</v>
       </c>
-      <c r="Q27" s="38">
+      <c r="Q27" s="36">
         <f t="shared" si="12"/>
         <v>2.1007460308194448E-2</v>
       </c>
-      <c r="R27" s="36">
+      <c r="R27" s="34">
         <f t="shared" si="13"/>
         <v>9.3368600865873717</v>
       </c>
-      <c r="S27" s="36">
+      <c r="S27" s="34">
         <f t="shared" si="14"/>
         <v>-1.1378227070112636</v>
       </c>
-      <c r="T27" s="39">
+      <c r="T27" s="37">
         <f t="shared" si="15"/>
         <v>-0.13877515790397443</v>
       </c>
@@ -3437,79 +3423,79 @@
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A28" s="35">
+      <c r="A28" s="33">
         <v>5</v>
       </c>
-      <c r="B28" s="53" t="s">
+      <c r="B28" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="36">
+      <c r="C28" s="34">
         <v>8.5018009823182705</v>
       </c>
-      <c r="D28" s="36">
+      <c r="D28" s="34">
         <v>0.18190417941925968</v>
       </c>
-      <c r="E28" s="38">
+      <c r="E28" s="36">
         <f t="shared" si="0"/>
         <v>2.1395958314900248E-2</v>
       </c>
-      <c r="F28" s="37">
+      <c r="F28" s="35">
         <f t="shared" si="1"/>
         <v>8.6222809885129195</v>
       </c>
-      <c r="G28" s="36">
+      <c r="G28" s="34">
         <f t="shared" si="2"/>
         <v>-0.12048000619464894</v>
       </c>
-      <c r="H28" s="38">
+      <c r="H28" s="36">
         <f t="shared" si="3"/>
         <v>-1.4171115795961198E-2</v>
       </c>
-      <c r="I28" s="37">
+      <c r="I28" s="35">
         <f t="shared" si="4"/>
         <v>8.7246005869276821</v>
       </c>
-      <c r="J28" s="36">
+      <c r="J28" s="34">
         <f t="shared" si="5"/>
         <v>-0.22279960460941162</v>
       </c>
-      <c r="K28" s="38">
+      <c r="K28" s="36">
         <f t="shared" si="6"/>
         <v>-2.6206165619823585E-2</v>
       </c>
-      <c r="L28" s="37">
+      <c r="L28" s="35">
         <f t="shared" si="7"/>
         <v>8.008926373128304</v>
       </c>
-      <c r="M28" s="36">
+      <c r="M28" s="34">
         <f t="shared" si="8"/>
         <v>0.49287460918996651</v>
       </c>
-      <c r="N28" s="38">
+      <c r="N28" s="36">
         <f t="shared" si="9"/>
         <v>5.7972964812400218E-2</v>
       </c>
-      <c r="O28" s="37">
+      <c r="O28" s="35">
         <f t="shared" si="10"/>
         <v>8.4471994025161017</v>
       </c>
-      <c r="P28" s="36">
+      <c r="P28" s="34">
         <f t="shared" si="11"/>
         <v>5.4601579802168843E-2</v>
       </c>
-      <c r="Q28" s="38">
+      <c r="Q28" s="36">
         <f t="shared" si="12"/>
         <v>6.4223545006202309E-3</v>
       </c>
-      <c r="R28" s="36">
+      <c r="R28" s="34">
         <f t="shared" si="13"/>
         <v>9.0949931620531714</v>
       </c>
-      <c r="S28" s="36">
+      <c r="S28" s="34">
         <f t="shared" si="14"/>
         <v>-0.5931921797349009</v>
       </c>
-      <c r="T28" s="39">
+      <c r="T28" s="37">
         <f t="shared" si="15"/>
         <v>-6.9772531839853658E-2</v>
       </c>
@@ -3530,79 +3516,79 @@
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A29" s="35">
+      <c r="A29" s="33">
         <v>5</v>
       </c>
-      <c r="B29" s="53" t="s">
+      <c r="B29" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="36">
+      <c r="C29" s="34">
         <v>8.0954876404494378</v>
       </c>
-      <c r="D29" s="36">
+      <c r="D29" s="34">
         <v>0.2954154330728892</v>
       </c>
-      <c r="E29" s="38">
+      <c r="E29" s="36">
         <f t="shared" si="0"/>
         <v>3.6491369784425812E-2</v>
       </c>
-      <c r="F29" s="37">
+      <c r="F29" s="35">
         <f t="shared" si="1"/>
         <v>7.7704354500513801</v>
       </c>
-      <c r="G29" s="36">
+      <c r="G29" s="34">
         <f t="shared" si="2"/>
         <v>0.32505219039805766</v>
       </c>
-      <c r="H29" s="38">
+      <c r="H29" s="36">
         <f t="shared" si="3"/>
         <v>4.0152268131930846E-2</v>
       </c>
-      <c r="I29" s="37">
+      <c r="I29" s="35">
         <f t="shared" si="4"/>
         <v>7.7833308673787407</v>
       </c>
-      <c r="J29" s="36">
+      <c r="J29" s="34">
         <f t="shared" si="5"/>
         <v>0.31215677307069711</v>
       </c>
-      <c r="K29" s="38">
+      <c r="K29" s="36">
         <f t="shared" si="6"/>
         <v>3.8559353918470984E-2</v>
       </c>
-      <c r="L29" s="37">
+      <c r="L29" s="35">
         <f t="shared" si="7"/>
         <v>7.3088548346667652</v>
       </c>
-      <c r="M29" s="36">
+      <c r="M29" s="34">
         <f t="shared" si="8"/>
         <v>0.78663280578267258</v>
       </c>
-      <c r="N29" s="38">
+      <c r="N29" s="36">
         <f t="shared" si="9"/>
         <v>9.7169292415719255E-2</v>
       </c>
-      <c r="O29" s="37">
+      <c r="O29" s="35">
         <f t="shared" si="10"/>
         <v>7.6833852377524314</v>
       </c>
-      <c r="P29" s="36">
+      <c r="P29" s="34">
         <f t="shared" si="11"/>
         <v>0.41210240269700638</v>
       </c>
-      <c r="Q29" s="38">
+      <c r="Q29" s="36">
         <f t="shared" si="12"/>
         <v>5.0905198179528988E-2</v>
       </c>
-      <c r="R29" s="36">
+      <c r="R29" s="34">
         <f t="shared" si="13"/>
         <v>8.6625597651092612</v>
       </c>
-      <c r="S29" s="36">
+      <c r="S29" s="34">
         <f t="shared" si="14"/>
         <v>-0.56707212465982337</v>
       </c>
-      <c r="T29" s="39">
+      <c r="T29" s="37">
         <f t="shared" si="15"/>
         <v>-7.0047926677872185E-2</v>
       </c>
@@ -3623,79 +3609,79 @@
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A30" s="35">
+      <c r="A30" s="33">
         <v>5</v>
       </c>
-      <c r="B30" s="53" t="s">
+      <c r="B30" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="36">
+      <c r="C30" s="34">
         <v>8.5194595330739293</v>
       </c>
-      <c r="D30" s="36">
+      <c r="D30" s="34">
         <v>0.3111203682459977</v>
       </c>
-      <c r="E30" s="38">
+      <c r="E30" s="36">
         <f t="shared" si="0"/>
         <v>3.6518791718908664E-2</v>
       </c>
-      <c r="F30" s="37">
+      <c r="F30" s="35">
         <f t="shared" ref="F30:F31" si="106">$C$1+X30</f>
         <v>7.9046312256634916</v>
       </c>
-      <c r="G30" s="36">
+      <c r="G30" s="34">
         <f t="shared" ref="G30" si="107">$C30-F30</f>
         <v>0.6148283074104377</v>
       </c>
-      <c r="H30" s="38">
+      <c r="H30" s="36">
         <f t="shared" ref="H30" si="108">1-F30/$C30</f>
         <v>7.2167524832247198E-2</v>
       </c>
-      <c r="I30" s="37">
+      <c r="I30" s="35">
         <f t="shared" si="4"/>
         <v>7.9046312256634916</v>
       </c>
-      <c r="J30" s="36">
+      <c r="J30" s="34">
         <f t="shared" si="5"/>
         <v>0.6148283074104377</v>
       </c>
-      <c r="K30" s="38">
+      <c r="K30" s="36">
         <f t="shared" si="6"/>
         <v>7.2167524832247198E-2</v>
       </c>
-      <c r="L30" s="37">
+      <c r="L30" s="35">
         <f t="shared" ref="L30:L31" si="109">$C$1+Z30</f>
         <v>7.2769852962052211</v>
       </c>
-      <c r="M30" s="36">
+      <c r="M30" s="34">
         <f t="shared" ref="M30" si="110">$C30-L30</f>
         <v>1.2424742368687083</v>
       </c>
-      <c r="N30" s="38">
+      <c r="N30" s="36">
         <f t="shared" ref="N30" si="111">1-L30/$C30</f>
         <v>0.14583956083660243</v>
       </c>
-      <c r="O30" s="37">
+      <c r="O30" s="35">
         <f t="shared" ref="O30:O31" si="112">$C$1+AA30</f>
         <v>7.6493222801148413</v>
       </c>
-      <c r="P30" s="36">
+      <c r="P30" s="34">
         <f t="shared" ref="P30" si="113">$C30-O30</f>
         <v>0.87013725295908806</v>
       </c>
-      <c r="Q30" s="38">
+      <c r="Q30" s="36">
         <f t="shared" ref="Q30" si="114">1-O30/$C30</f>
         <v>0.10213526451778698</v>
       </c>
-      <c r="R30" s="36">
+      <c r="R30" s="34">
         <f t="shared" ref="R30:R31" si="115">$C$1+AB30</f>
         <v>8.7058591417414206</v>
       </c>
-      <c r="S30" s="36">
+      <c r="S30" s="34">
         <f t="shared" ref="S30" si="116">$C30-R30</f>
         <v>-0.18639960866749128</v>
       </c>
-      <c r="T30" s="39">
+      <c r="T30" s="37">
         <f t="shared" ref="T30" si="117">1-R30/$C30</f>
         <v>-2.1879276255008628E-2</v>
       </c>
@@ -3716,79 +3702,79 @@
       </c>
     </row>
     <row r="31" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="40">
+      <c r="A31" s="38">
         <v>5</v>
       </c>
-      <c r="B31" s="54" t="s">
+      <c r="B31" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="41">
+      <c r="C31" s="39">
         <v>8.1599680170575706</v>
       </c>
-      <c r="D31" s="41">
+      <c r="D31" s="39">
         <v>0.35412005679911923</v>
       </c>
-      <c r="E31" s="43">
+      <c r="E31" s="41">
         <f t="shared" si="0"/>
         <v>4.3397235878727444E-2</v>
       </c>
-      <c r="F31" s="42">
+      <c r="F31" s="40">
         <f t="shared" si="106"/>
         <v>7.779321616548641</v>
       </c>
-      <c r="G31" s="41">
+      <c r="G31" s="39">
         <f t="shared" ref="G31" si="118">$C31-F31</f>
         <v>0.38064640050892962</v>
       </c>
-      <c r="H31" s="43">
+      <c r="H31" s="41">
         <f t="shared" ref="H31" si="119">1-F31/$C31</f>
         <v>4.664802603554663E-2</v>
       </c>
-      <c r="I31" s="41">
+      <c r="I31" s="39">
         <f t="shared" si="4"/>
         <v>7.7888339242409508</v>
       </c>
-      <c r="J31" s="41">
+      <c r="J31" s="39">
         <f t="shared" ref="J31" si="120">$C31-I31</f>
         <v>0.3711340928166198</v>
       </c>
-      <c r="K31" s="43">
+      <c r="K31" s="41">
         <f t="shared" ref="K31" si="121">1-I31/$C31</f>
         <v>4.5482297484598311E-2</v>
       </c>
-      <c r="L31" s="42">
+      <c r="L31" s="40">
         <f t="shared" si="109"/>
         <v>7.3088548346667608</v>
       </c>
-      <c r="M31" s="41">
+      <c r="M31" s="39">
         <f t="shared" ref="M31" si="122">$C31-L31</f>
         <v>0.8511131823908098</v>
       </c>
-      <c r="N31" s="43">
+      <c r="N31" s="41">
         <f t="shared" ref="N31" si="123">1-L31/$C31</f>
         <v>0.10430349489258361</v>
       </c>
-      <c r="O31" s="42">
+      <c r="O31" s="40">
         <f t="shared" si="112"/>
         <v>7.7027269300601215</v>
       </c>
-      <c r="P31" s="41">
+      <c r="P31" s="39">
         <f t="shared" ref="P31" si="124">$C31-O31</f>
         <v>0.45724108699744903</v>
       </c>
-      <c r="Q31" s="43">
+      <c r="Q31" s="41">
         <f t="shared" ref="Q31" si="125">1-O31/$C31</f>
         <v>5.603466656261813E-2</v>
       </c>
-      <c r="R31" s="41">
+      <c r="R31" s="39">
         <f t="shared" si="115"/>
         <v>8.7012431497246414</v>
       </c>
-      <c r="S31" s="41">
+      <c r="S31" s="39">
         <f t="shared" ref="S31" si="126">$C31-R31</f>
         <v>-0.54127513266707084</v>
       </c>
-      <c r="T31" s="44">
+      <c r="T31" s="42">
         <f t="shared" ref="T31" si="127">1-R31/$C31</f>
         <v>-6.6332996837192404E-2</v>
       </c>
@@ -3809,326 +3795,326 @@
       </c>
     </row>
     <row r="32" spans="1:28" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="67" t="s">
+      <c r="A32" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="68"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="56">
-        <f>AVERAGE(G7:G30)</f>
-        <v>0.15564711144482712</v>
-      </c>
-      <c r="H32" s="59">
-        <f>AVERAGE(H7:H30)</f>
-        <v>1.8331254193035256E-2</v>
-      </c>
-      <c r="I32" s="63"/>
-      <c r="J32" s="56">
-        <f>AVERAGE(J7:J30)</f>
-        <v>0.10882692593161362</v>
-      </c>
-      <c r="K32" s="59">
-        <f>AVERAGE(K7:K30)</f>
-        <v>1.2551653923119466E-2</v>
-      </c>
-      <c r="L32" s="58"/>
-      <c r="M32" s="56">
-        <f>AVERAGE(M7:M30)</f>
-        <v>0.68604247583265432</v>
-      </c>
-      <c r="N32" s="59">
-        <f>AVERAGE(N7:N30)</f>
-        <v>8.4083995042370796E-2</v>
-      </c>
-      <c r="O32" s="58"/>
-      <c r="P32" s="56">
-        <f>AVERAGE(P7:P30)</f>
-        <v>0.29546928901614983</v>
-      </c>
-      <c r="Q32" s="59">
-        <f>AVERAGE(Q7:Q30)</f>
-        <v>3.550213585938608E-2</v>
-      </c>
-      <c r="R32" s="56"/>
-      <c r="S32" s="56">
-        <f>AVERAGE(S7:S30)</f>
-        <v>-0.60717999781679355</v>
-      </c>
-      <c r="T32" s="60">
-        <f>AVERAGE(T7:T30)</f>
-        <v>-7.7276704575810609E-2</v>
+      <c r="B32" s="78"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="54">
+        <f>AVERAGE(G7:G31)</f>
+        <v>0.16464708300739123</v>
+      </c>
+      <c r="H32" s="57">
+        <f>AVERAGE(H7:H31)</f>
+        <v>1.9463925066735711E-2</v>
+      </c>
+      <c r="I32" s="60"/>
+      <c r="J32" s="54">
+        <f>AVERAGE(J7:J31)</f>
+        <v>0.11931921260701386</v>
+      </c>
+      <c r="K32" s="57">
+        <f>AVERAGE(K7:K31)</f>
+        <v>1.3868879665578619E-2</v>
+      </c>
+      <c r="L32" s="56"/>
+      <c r="M32" s="54">
+        <f>AVERAGE(M7:M31)</f>
+        <v>0.6926453040949806</v>
+      </c>
+      <c r="N32" s="57">
+        <f>AVERAGE(N7:N31)</f>
+        <v>8.4892775036379306E-2</v>
+      </c>
+      <c r="O32" s="56"/>
+      <c r="P32" s="54">
+        <f>AVERAGE(P7:P31)</f>
+        <v>0.30194016093540177</v>
+      </c>
+      <c r="Q32" s="57">
+        <f>AVERAGE(Q7:Q31)</f>
+        <v>3.6323437087515363E-2</v>
+      </c>
+      <c r="R32" s="54"/>
+      <c r="S32" s="54">
+        <f>AVERAGE(S7:S31)</f>
+        <v>-0.60454380321080459</v>
+      </c>
+      <c r="T32" s="57">
+        <f>AVERAGE(T7:T31)</f>
+        <v>-7.6838956266265884E-2</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="67" t="s">
+      <c r="A33" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="68"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="56">
-        <f>_xlfn.STDEV.P(G7:G30)</f>
-        <v>0.25545565530404024</v>
-      </c>
-      <c r="H33" s="59">
-        <f>_xlfn.STDEV.P(H7:H30)</f>
-        <v>3.1727366009334367E-2</v>
-      </c>
-      <c r="I33" s="63"/>
-      <c r="J33" s="56">
-        <f>_xlfn.STDEV.P(J7:J30)</f>
-        <v>0.27043601743686524</v>
-      </c>
-      <c r="K33" s="59">
-        <f>_xlfn.STDEV.P(K7:K30)</f>
-        <v>3.3897593157115803E-2</v>
-      </c>
-      <c r="L33" s="58"/>
-      <c r="M33" s="56">
-        <f>_xlfn.STDEV.P(M7:M30)</f>
-        <v>0.27677271401471298</v>
-      </c>
-      <c r="N33" s="59">
-        <f>_xlfn.STDEV.P(N7:N30)</f>
-        <v>3.1945685834260849E-2</v>
-      </c>
-      <c r="O33" s="58"/>
-      <c r="P33" s="56">
-        <f>_xlfn.STDEV.P(P7:P30)</f>
-        <v>0.25896554909331332</v>
-      </c>
-      <c r="Q33" s="59">
-        <f>_xlfn.STDEV.P(Q7:Q30)</f>
-        <v>3.1078841234699738E-2</v>
-      </c>
-      <c r="R33" s="56"/>
-      <c r="S33" s="56">
-        <f>_xlfn.STDEV.P(S7:S30)</f>
-        <v>0.36417381317576536</v>
-      </c>
-      <c r="T33" s="60">
-        <f>_xlfn.STDEV.P(T7:T30)</f>
-        <v>4.6541692148518783E-2</v>
+      <c r="B33" s="78"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="54">
+        <f>_xlfn.STDEV.P(G7:G31)</f>
+        <v>0.25414813764572636</v>
+      </c>
+      <c r="H33" s="57">
+        <f>_xlfn.STDEV.P(H7:H31)</f>
+        <v>3.1577703575937248E-2</v>
+      </c>
+      <c r="I33" s="60"/>
+      <c r="J33" s="54">
+        <f>_xlfn.STDEV.P(J7:J31)</f>
+        <v>0.26991170381870944</v>
+      </c>
+      <c r="K33" s="57">
+        <f>_xlfn.STDEV.P(K7:K31)</f>
+        <v>3.3833813807046045E-2</v>
+      </c>
+      <c r="L33" s="56"/>
+      <c r="M33" s="54">
+        <f>_xlfn.STDEV.P(M7:M31)</f>
+        <v>0.27310317830378644</v>
+      </c>
+      <c r="N33" s="57">
+        <f>_xlfn.STDEV.P(N7:N31)</f>
+        <v>3.155003599955862E-2</v>
+      </c>
+      <c r="O33" s="56"/>
+      <c r="P33" s="54">
+        <f>_xlfn.STDEV.P(P7:P31)</f>
+        <v>0.25570600656613829</v>
+      </c>
+      <c r="Q33" s="57">
+        <f>_xlfn.STDEV.P(Q7:Q31)</f>
+        <v>3.0715589764284942E-2</v>
+      </c>
+      <c r="R33" s="54"/>
+      <c r="S33" s="54">
+        <f>_xlfn.STDEV.P(S7:S31)</f>
+        <v>0.35704964932467542</v>
+      </c>
+      <c r="T33" s="57">
+        <f>_xlfn.STDEV.P(T7:T31)</f>
+        <v>4.5651756918061955E-2</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A34" s="69" t="s">
+      <c r="A34" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="70"/>
+      <c r="B34" s="80"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="12"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="10"/>
       <c r="G34" s="5" cm="1">
-        <f t="array" ref="G34">AVERAGE(ABS(G7:G30))</f>
-        <v>0.25160288580601986</v>
-      </c>
-      <c r="H34" s="11" cm="1">
-        <f t="array" ref="H34">AVERAGE(ABS(H7:H30))</f>
-        <v>3.0957498557189267E-2</v>
-      </c>
-      <c r="I34" s="64"/>
+        <f t="array" ref="G34">AVERAGE(ABS(G7:G31))</f>
+        <v>0.25676462639413627</v>
+      </c>
+      <c r="H34" s="9" cm="1">
+        <f t="array" ref="H34">AVERAGE(ABS(H7:H31))</f>
+        <v>3.158511965632356E-2</v>
+      </c>
+      <c r="I34" s="61"/>
       <c r="J34" s="5" cm="1">
-        <f t="array" ref="J34">AVERAGE(ABS(J7:J30))</f>
-        <v>0.2414821652562337</v>
-      </c>
-      <c r="K34" s="11" cm="1">
-        <f t="array" ref="K34">AVERAGE(ABS(K7:K30))</f>
-        <v>2.9834314346570801E-2</v>
-      </c>
-      <c r="L34" s="12"/>
+        <f t="array" ref="J34">AVERAGE(ABS(J7:J31))</f>
+        <v>0.24666824235864915</v>
+      </c>
+      <c r="K34" s="9" cm="1">
+        <f t="array" ref="K34">AVERAGE(ABS(K7:K31))</f>
+        <v>3.0460233672091899E-2</v>
+      </c>
+      <c r="L34" s="10"/>
       <c r="M34" s="5" cm="1">
-        <f t="array" ref="M34">AVERAGE(ABS(M7:M30))</f>
-        <v>0.68604247583265432</v>
-      </c>
-      <c r="N34" s="11" cm="1">
-        <f t="array" ref="N34">AVERAGE(ABS(N7:N30))</f>
-        <v>8.4083995042370796E-2</v>
-      </c>
-      <c r="O34" s="12"/>
+        <f t="array" ref="M34">AVERAGE(ABS(M7:M31))</f>
+        <v>0.6926453040949806</v>
+      </c>
+      <c r="N34" s="9" cm="1">
+        <f t="array" ref="N34">AVERAGE(ABS(N7:N31))</f>
+        <v>8.4892775036379306E-2</v>
+      </c>
+      <c r="O34" s="10"/>
       <c r="P34" s="5" cm="1">
-        <f t="array" ref="P34">AVERAGE(ABS(P7:P30))</f>
-        <v>0.32856736990360152</v>
-      </c>
-      <c r="Q34" s="11" cm="1">
-        <f t="array" ref="Q34">AVERAGE(ABS(Q7:Q30))</f>
-        <v>4.0002267381755004E-2</v>
+        <f t="array" ref="P34">AVERAGE(ABS(P7:P31))</f>
+        <v>0.3337143185873554</v>
+      </c>
+      <c r="Q34" s="9" cm="1">
+        <f t="array" ref="Q34">AVERAGE(ABS(Q7:Q31))</f>
+        <v>4.0643563348989532E-2</v>
       </c>
       <c r="R34" s="4"/>
       <c r="S34" s="5" cm="1">
-        <f t="array" ref="S34">AVERAGE(ABS(S7:S30))</f>
-        <v>0.64258806149266912</v>
-      </c>
-      <c r="T34" s="6" cm="1">
-        <f t="array" ref="T34">AVERAGE(ABS(T7:T30))</f>
-        <v>8.1277713810838856E-2</v>
+        <f t="array" ref="S34">AVERAGE(ABS(S7:S31))</f>
+        <v>0.63853554433964521</v>
+      </c>
+      <c r="T34" s="9" cm="1">
+        <f t="array" ref="T34">AVERAGE(ABS(T7:T31))</f>
+        <v>8.0679925131892996E-2</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A35" s="69" t="s">
+      <c r="A35" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="70"/>
+      <c r="B35" s="80"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="12"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="10"/>
       <c r="G35" s="5" cm="1">
-        <f t="array" ref="G35">_xlfn.STDEV.P(ABS(G7:G30))</f>
-        <v>0.16180112169579666</v>
-      </c>
-      <c r="H35" s="11" cm="1">
-        <f t="array" ref="H35">_xlfn.STDEV.P(ABS(H7:H30))</f>
-        <v>1.9603415958999667E-2</v>
-      </c>
-      <c r="I35" s="64"/>
+        <f t="array" ref="G35">_xlfn.STDEV.P(ABS(G7:G31))</f>
+        <v>0.16053617799210704</v>
+      </c>
+      <c r="H35" s="9" cm="1">
+        <f t="array" ref="H35">_xlfn.STDEV.P(ABS(H7:H31))</f>
+        <v>1.9451888299828003E-2</v>
+      </c>
+      <c r="I35" s="61"/>
       <c r="J35" s="5" cm="1">
-        <f t="array" ref="J35">_xlfn.STDEV.P(ABS(J7:J30))</f>
-        <v>0.16329514137903314</v>
-      </c>
-      <c r="K35" s="11" cm="1">
-        <f t="array" ref="K35">_xlfn.STDEV.P(ABS(K7:K30))</f>
-        <v>2.0408442506009716E-2</v>
-      </c>
-      <c r="L35" s="12"/>
+        <f t="array" ref="J35">_xlfn.STDEV.P(ABS(J7:J31))</f>
+        <v>0.16200055730512544</v>
+      </c>
+      <c r="K35" s="9" cm="1">
+        <f t="array" ref="K35">_xlfn.STDEV.P(ABS(K7:K31))</f>
+        <v>2.0229852805933084E-2</v>
+      </c>
+      <c r="L35" s="10"/>
       <c r="M35" s="5" cm="1">
-        <f t="array" ref="M35">_xlfn.STDEV.P(ABS(M7:M30))</f>
-        <v>0.27677271401471298</v>
-      </c>
-      <c r="N35" s="11" cm="1">
-        <f t="array" ref="N35">_xlfn.STDEV.P(ABS(N7:N30))</f>
-        <v>3.1945685834260849E-2</v>
-      </c>
-      <c r="O35" s="12"/>
+        <f t="array" ref="M35">_xlfn.STDEV.P(ABS(M7:M31))</f>
+        <v>0.27310317830378644</v>
+      </c>
+      <c r="N35" s="9" cm="1">
+        <f t="array" ref="N35">_xlfn.STDEV.P(ABS(N7:N31))</f>
+        <v>3.155003599955862E-2</v>
+      </c>
+      <c r="O35" s="10"/>
       <c r="P35" s="5" cm="1">
-        <f t="array" ref="P35">_xlfn.STDEV.P(ABS(P7:P30))</f>
-        <v>0.21542687808985267</v>
-      </c>
-      <c r="Q35" s="11" cm="1">
-        <f t="array" ref="Q35">_xlfn.STDEV.P(ABS(Q7:Q30))</f>
-        <v>2.5022282617470359E-2</v>
+        <f t="array" ref="P35">_xlfn.STDEV.P(ABS(P7:P31))</f>
+        <v>0.21257510707859315</v>
+      </c>
+      <c r="Q35" s="9" cm="1">
+        <f t="array" ref="Q35">_xlfn.STDEV.P(ABS(Q7:Q31))</f>
+        <v>2.4717206450471044E-2</v>
       </c>
       <c r="R35" s="4"/>
       <c r="S35" s="5" cm="1">
-        <f t="array" ref="S35">_xlfn.STDEV.P(ABS(S7:S30))</f>
-        <v>0.29727209619954637</v>
-      </c>
-      <c r="T35" s="6" cm="1">
-        <f t="array" ref="T35">_xlfn.STDEV.P(ABS(T7:T30))</f>
-        <v>3.9137595938278827E-2</v>
+        <f t="array" ref="S35">_xlfn.STDEV.P(ABS(S7:S31))</f>
+        <v>0.29194181046628243</v>
+      </c>
+      <c r="T35" s="9" cm="1">
+        <f t="array" ref="T35">_xlfn.STDEV.P(ABS(T7:T31))</f>
+        <v>3.845852038894737E-2</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A36" s="69" t="s">
+      <c r="A36" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="70"/>
+      <c r="B36" s="80"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="12"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="10"/>
       <c r="G36" s="5" cm="1">
-        <f t="array" ref="G36">MAX(ABS(G7:G30))</f>
+        <f t="array" ref="G36">MAX(ABS(G7:G31))</f>
         <v>0.6148283074104377</v>
       </c>
-      <c r="H36" s="11" cm="1">
-        <f t="array" ref="H36">MAX(ABS(H7:H30))</f>
+      <c r="H36" s="9" cm="1">
+        <f t="array" ref="H36">MAX(ABS(H7:H31))</f>
         <v>7.5533209795243472E-2</v>
       </c>
-      <c r="I36" s="64"/>
+      <c r="I36" s="61"/>
       <c r="J36" s="5" cm="1">
-        <f t="array" ref="J36">MAX(ABS(J7:J30))</f>
+        <f t="array" ref="J36">MAX(ABS(J7:J31))</f>
         <v>0.66337765838167329</v>
       </c>
-      <c r="K36" s="11" cm="1">
-        <f t="array" ref="K36">MAX(ABS(K7:K30))</f>
+      <c r="K36" s="9" cm="1">
+        <f t="array" ref="K36">MAX(ABS(K7:K31))</f>
         <v>8.8887849436025679E-2</v>
       </c>
-      <c r="L36" s="12"/>
+      <c r="L36" s="10"/>
       <c r="M36" s="5" cm="1">
-        <f t="array" ref="M36">MAX(ABS(M7:M30))</f>
+        <f t="array" ref="M36">MAX(ABS(M7:M31))</f>
         <v>1.2424742368687083</v>
       </c>
-      <c r="N36" s="11" cm="1">
-        <f t="array" ref="N36">MAX(ABS(N7:N30))</f>
+      <c r="N36" s="9" cm="1">
+        <f t="array" ref="N36">MAX(ABS(N7:N31))</f>
         <v>0.14583956083660243</v>
       </c>
-      <c r="O36" s="12"/>
+      <c r="O36" s="10"/>
       <c r="P36" s="5" cm="1">
-        <f t="array" ref="P36">MAX(ABS(P7:P30))</f>
+        <f t="array" ref="P36">MAX(ABS(P7:P31))</f>
         <v>0.87013725295908806</v>
       </c>
-      <c r="Q36" s="11" cm="1">
-        <f t="array" ref="Q36">MAX(ABS(Q7:Q30))</f>
+      <c r="Q36" s="9" cm="1">
+        <f t="array" ref="Q36">MAX(ABS(Q7:Q31))</f>
         <v>0.10213526451778698</v>
       </c>
       <c r="R36" s="4"/>
       <c r="S36" s="5" cm="1">
-        <f t="array" ref="S36">MAX(ABS(S7:S30))</f>
+        <f t="array" ref="S36">MAX(ABS(S7:S31))</f>
         <v>1.1378227070112636</v>
       </c>
-      <c r="T36" s="6" cm="1">
-        <f t="array" ref="T36">MAX(ABS(T7:T30))</f>
+      <c r="T36" s="9" cm="1">
+        <f t="array" ref="T36">MAX(ABS(T7:T31))</f>
         <v>0.13877515790397443</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="71" t="s">
+      <c r="A37" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="72"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="13"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="11"/>
       <c r="G37" s="1" cm="1">
-        <f t="array" ref="G37">MIN(ABS(G7:G30))</f>
+        <f t="array" ref="G37">MIN(ABS(G7:G31))</f>
         <v>1.4130608936810063E-2</v>
       </c>
-      <c r="H37" s="14" cm="1">
-        <f t="array" ref="H37">MIN(ABS(H7:H30))</f>
+      <c r="H37" s="12" cm="1">
+        <f t="array" ref="H37">MIN(ABS(H7:H31))</f>
         <v>1.7234473124869698E-3</v>
       </c>
-      <c r="I37" s="65"/>
+      <c r="I37" s="62"/>
       <c r="J37" s="1" cm="1">
-        <f t="array" ref="J37">MIN(ABS(J7:J30))</f>
+        <f t="array" ref="J37">MIN(ABS(J7:J31))</f>
         <v>3.4882595438698871E-3</v>
       </c>
-      <c r="K37" s="14" cm="1">
-        <f t="array" ref="K37">MIN(ABS(K7:K30))</f>
+      <c r="K37" s="12" cm="1">
+        <f t="array" ref="K37">MIN(ABS(K7:K31))</f>
         <v>4.6443153797137704E-4</v>
       </c>
-      <c r="L37" s="13"/>
+      <c r="L37" s="11"/>
       <c r="M37" s="1" cm="1">
-        <f t="array" ref="M37">MIN(ABS(M7:M30))</f>
+        <f t="array" ref="M37">MIN(ABS(M7:M31))</f>
         <v>0.16327629845039571</v>
       </c>
-      <c r="N37" s="14" cm="1">
-        <f t="array" ref="N37">MIN(ABS(N7:N30))</f>
+      <c r="N37" s="12" cm="1">
+        <f t="array" ref="N37">MIN(ABS(N7:N31))</f>
         <v>2.2563181005000876E-2</v>
       </c>
-      <c r="O37" s="13"/>
+      <c r="O37" s="11"/>
       <c r="P37" s="1" cm="1">
-        <f t="array" ref="P37">MIN(ABS(P7:P30))</f>
+        <f t="array" ref="P37">MIN(ABS(P7:P31))</f>
         <v>1.8250825119585201E-2</v>
       </c>
-      <c r="Q37" s="14" cm="1">
-        <f t="array" ref="Q37">MIN(ABS(Q7:Q30))</f>
+      <c r="Q37" s="12" cm="1">
+        <f t="array" ref="Q37">MIN(ABS(Q7:Q31))</f>
         <v>2.240271085906409E-3</v>
       </c>
-      <c r="R37" s="7"/>
+      <c r="R37" s="6"/>
       <c r="S37" s="1" cm="1">
-        <f t="array" ref="S37">MIN(ABS(S7:S30))</f>
+        <f t="array" ref="S37">MIN(ABS(S7:S31))</f>
         <v>2.8329665201379584E-2</v>
       </c>
-      <c r="T37" s="8" cm="1">
-        <f t="array" ref="T37">MIN(ABS(T7:T30))</f>
+      <c r="T37" s="12" cm="1">
+        <f t="array" ref="T37">MIN(ABS(T7:T31))</f>
         <v>3.150812184177898E-3</v>
       </c>
     </row>
@@ -4166,6 +4152,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A33:B33"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="L5:N5"/>
@@ -4176,12 +4168,6 @@
     <mergeCell ref="C4:E5"/>
     <mergeCell ref="F4:T4"/>
     <mergeCell ref="I5:K5"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A33:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="61" orientation="landscape" r:id="rId1"/>
@@ -4200,7 +4186,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="63" t="s">
         <v>32</v>
       </c>
       <c r="H1">
@@ -4209,7 +4195,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="63" t="s">
         <v>33</v>
       </c>
       <c r="H2">
@@ -4218,7 +4204,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="63" t="s">
         <v>34</v>
       </c>
       <c r="H3">
@@ -4227,7 +4213,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="63" t="s">
         <v>35</v>
       </c>
       <c r="H4">
@@ -4236,7 +4222,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="63" t="s">
         <v>36</v>
       </c>
       <c r="H5">
@@ -4245,7 +4231,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="63" t="s">
         <v>37</v>
       </c>
       <c r="H6">
@@ -4254,7 +4240,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="63" t="s">
         <v>38</v>
       </c>
       <c r="H7">
@@ -4263,7 +4249,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="63" t="s">
         <v>39</v>
       </c>
       <c r="H8">
@@ -4272,7 +4258,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="63" t="s">
         <v>40</v>
       </c>
       <c r="H9">
@@ -4281,7 +4267,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="63" t="s">
         <v>41</v>
       </c>
       <c r="H10">
@@ -4290,7 +4276,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="63" t="s">
         <v>43</v>
       </c>
       <c r="H11">
@@ -4299,7 +4285,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="63" t="s">
         <v>42</v>
       </c>
       <c r="H12">
@@ -4308,7 +4294,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="63" t="s">
         <v>44</v>
       </c>
       <c r="H13">
@@ -4317,7 +4303,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="66" t="s">
+      <c r="A14" s="63" t="s">
         <v>45</v>
       </c>
       <c r="H14">
@@ -4326,7 +4312,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="63" t="s">
         <v>46</v>
       </c>
       <c r="H15">
@@ -4335,7 +4321,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="63" t="s">
         <v>47</v>
       </c>
       <c r="H16">
@@ -4344,7 +4330,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="63" t="s">
         <v>48</v>
       </c>
       <c r="H17">
@@ -4353,7 +4339,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="63" t="s">
         <v>49</v>
       </c>
       <c r="H18">
@@ -4362,7 +4348,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="63" t="s">
         <v>51</v>
       </c>
       <c r="H19">
@@ -4371,7 +4357,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="63" t="s">
         <v>50</v>
       </c>
       <c r="H20">

</xml_diff>